<commit_message>
Actualizacion plantilla plan de proyecto
</commit_message>
<xml_diff>
--- a/Organización/Planeación/PTL_Plan_proyecto.xlsx
+++ b/Organización/Planeación/PTL_Plan_proyecto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Presentación" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,6 +31,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="Complej." vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="Complej." vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'Plan Riesgos'!$A$1:$F$24</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$24</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -997,7 +998,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="132">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1134,7 +1135,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1218,7 +1219,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1522,6 +1523,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1530,7 +1535,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="TableStyleLight1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -1601,15 +1606,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>378000</xdr:colOff>
+      <xdr:colOff>405000</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>84960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>378360</xdr:colOff>
+      <xdr:colOff>405360</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>94320</xdr:rowOff>
+      <xdr:rowOff>85320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1618,7 +1623,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6385680" y="2925360"/>
+          <a:off x="6412680" y="2916360"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1626,7 +1631,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:ln w="28440">
-          <a:round/>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -1641,15 +1646,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1116000</xdr:colOff>
+      <xdr:colOff>1143000</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>66600</xdr:rowOff>
+      <xdr:rowOff>57600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>985680</xdr:colOff>
+      <xdr:colOff>1012320</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>66960</xdr:rowOff>
+      <xdr:rowOff>57960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1658,8 +1663,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1116000" y="6740280"/>
-          <a:ext cx="5877360" cy="360"/>
+          <a:off x="1143000" y="6731280"/>
+          <a:ext cx="5877000" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1681,15 +1686,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>849600</xdr:colOff>
+      <xdr:colOff>876600</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>105120</xdr:rowOff>
+      <xdr:rowOff>96120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2341800</xdr:colOff>
+      <xdr:colOff>2368440</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>105480</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1698,8 +1703,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="849600" y="5483520"/>
-          <a:ext cx="11188440" cy="360"/>
+          <a:off x="876600" y="5474520"/>
+          <a:ext cx="11188080" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1707,516 +1712,6 @@
         <a:noFill/>
         <a:ln w="9360">
           <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>769680</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10035720" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>769680</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10035720" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>769680</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10035720" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>712440</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10037520" cy="9524160"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>712440</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10037520" cy="9524160"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>712440</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10037520" cy="9524160"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>712440</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10037520" cy="9524160"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>2284200</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="9946800" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>2284200</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="9946800" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>2284200</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="9946800" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>2284200</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="9946800" cy="9524520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2362,8 +1857,8 @@
   </sheetPr>
   <dimension ref="A1:AMI30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4686,8 +4181,8 @@
   </sheetPr>
   <dimension ref="1:23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -20161,6 +19656,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A22" s="0"/>
+      <c r="B22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A23" s="10"/>
@@ -20323,7 +19819,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -24556,8 +24052,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -24569,7 +24064,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -24768,8 +24263,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -24781,7 +24275,7 @@
   <dimension ref="1:43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -52967,9 +52461,11 @@
       <c r="AE40" s="56"/>
       <c r="AF40" s="56"/>
     </row>
-    <row r="41" s="129" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="55"/>
-      <c r="D41" s="55"/>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="129"/>
+      <c r="B41" s="129"/>
+      <c r="C41" s="131"/>
+      <c r="D41" s="131"/>
       <c r="G41" s="56"/>
       <c r="H41" s="56"/>
       <c r="I41" s="56"/>
@@ -52997,9 +52493,11 @@
       <c r="AE41" s="56"/>
       <c r="AF41" s="56"/>
     </row>
-    <row r="42" s="129" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="55"/>
-      <c r="D42" s="55"/>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="129"/>
+      <c r="B42" s="129"/>
+      <c r="C42" s="131"/>
+      <c r="D42" s="131"/>
       <c r="G42" s="56"/>
       <c r="H42" s="56"/>
       <c r="I42" s="56"/>
@@ -53027,9 +52525,11 @@
       <c r="AE42" s="56"/>
       <c r="AF42" s="56"/>
     </row>
-    <row r="43" s="129" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="55"/>
-      <c r="D43" s="55"/>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="129"/>
+      <c r="B43" s="129"/>
+      <c r="C43" s="131"/>
+      <c r="D43" s="131"/>
       <c r="G43" s="56"/>
       <c r="H43" s="56"/>
       <c r="I43" s="56"/>
@@ -53105,7 +52605,6 @@
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="24" man="true" max="16383" min="0"/>
   </rowBreaks>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Avtualizacion plan de proyecto
</commit_message>
<xml_diff>
--- a/Organización/Planeación/PTL_Plan_proyecto.xlsx
+++ b/Organización/Planeación/PTL_Plan_proyecto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Presentación" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,6 +32,7 @@
     <definedName function="false" hidden="false" localSheetId="6" name="Complej." vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'Plan Riesgos'!$A$1:$F$24</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$24</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$24</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -234,7 +235,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="104">
   <si>
     <t>Plan del Proyecto</t>
   </si>
@@ -511,6 +512,42 @@
   <si>
     <t>Alto</t>
   </si>
+  <si>
+    <t>Tabla descriptiva de prioridad</t>
+  </si>
+  <si>
+    <t>Nivel</t>
+  </si>
+  <si>
+    <t>Rango de exposición</t>
+  </si>
+  <si>
+    <t>Prioridad</t>
+  </si>
+  <si>
+    <t>1.81 o mayor</t>
+  </si>
+  <si>
+    <t>Urgente</t>
+  </si>
+  <si>
+    <t>1.21 – 1.80</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>0.61 – 1.20</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>0 – 0.60</t>
+  </si>
+  <si>
+    <t>Baja</t>
+  </si>
 </sst>
 </file>
 
@@ -695,7 +732,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -711,7 +748,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFEEEEEE"/>
       </patternFill>
     </fill>
     <fill>
@@ -735,7 +772,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFE6E6FF"/>
+        <bgColor rgb="FFEEEEEE"/>
       </patternFill>
     </fill>
     <fill>
@@ -786,8 +823,14 @@
         <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFE6E6FF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="27">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -963,6 +1006,20 @@
       <bottom style="medium"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -998,7 +1055,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="139">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1511,8 +1568,36 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="22" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="16" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="16" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="3" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="3" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="3" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="22" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1558,7 +1643,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF93CDDD"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFE6E6FF"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFCFE7F5"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -1578,7 +1663,7 @@
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFE6E6FF"/>
       <rgbColor rgb="FFD9D9D9"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
@@ -1606,15 +1691,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>405000</xdr:colOff>
+      <xdr:colOff>432000</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
+      <xdr:rowOff>75960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>405360</xdr:colOff>
+      <xdr:colOff>432360</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>76320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1623,7 +1708,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6412680" y="2916360"/>
+          <a:off x="6439680" y="2907360"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1646,15 +1731,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:colOff>1170000</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>57600</xdr:rowOff>
+      <xdr:rowOff>48600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1012320</xdr:colOff>
+      <xdr:colOff>1038960</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>57960</xdr:rowOff>
+      <xdr:rowOff>48960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1663,8 +1748,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1143000" y="6731280"/>
-          <a:ext cx="5877000" cy="360"/>
+          <a:off x="1170000" y="6722280"/>
+          <a:ext cx="5876640" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1686,15 +1771,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>876600</xdr:colOff>
+      <xdr:colOff>903600</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>96120</xdr:rowOff>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2368440</xdr:colOff>
+      <xdr:colOff>2395080</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>87480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1703,8 +1788,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="876600" y="5474520"/>
-          <a:ext cx="11188080" cy="360"/>
+          <a:off x="903600" y="5465520"/>
+          <a:ext cx="11187720" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4181,7 +4266,7 @@
   </sheetPr>
   <dimension ref="1:23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -19803,8 +19888,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -24274,8 +24359,8 @@
   </sheetPr>
   <dimension ref="1:43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -48269,9 +48354,11 @@
     </row>
     <row r="28" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="127"/>
-      <c r="B28" s="127"/>
-      <c r="C28" s="127"/>
-      <c r="D28" s="127"/>
+      <c r="B28" s="128"/>
+      <c r="C28" s="129" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="130"/>
       <c r="E28" s="127"/>
       <c r="F28" s="127"/>
       <c r="G28" s="0"/>
@@ -49293,11 +49380,17 @@
       <c r="AMI28" s="0"/>
       <c r="AMJ28" s="0"/>
     </row>
-    <row r="29" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="127"/>
-      <c r="B29" s="127"/>
-      <c r="C29" s="127"/>
-      <c r="D29" s="127"/>
+      <c r="B29" s="131" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="132" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="131" t="s">
+        <v>95</v>
+      </c>
       <c r="E29" s="127"/>
       <c r="F29" s="127"/>
       <c r="G29" s="0"/>
@@ -50321,10 +50414,16 @@
     </row>
     <row r="30" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="127"/>
-      <c r="B30" s="127"/>
-      <c r="C30" s="128"/>
-      <c r="D30" s="128"/>
-      <c r="E30" s="128"/>
+      <c r="B30" s="131" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="133" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="131" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" s="134"/>
       <c r="F30" s="127"/>
       <c r="G30" s="0"/>
       <c r="H30" s="0"/>
@@ -51345,11 +51444,17 @@
       <c r="AMI30" s="0"/>
       <c r="AMJ30" s="0"/>
     </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
-      <c r="B31" s="0"/>
-      <c r="C31" s="0"/>
-      <c r="D31" s="0"/>
+      <c r="B31" s="135" t="n">
+        <v>2</v>
+      </c>
+      <c r="C31" s="135" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="135" t="s">
+        <v>99</v>
+      </c>
       <c r="E31" s="0"/>
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
@@ -52371,9 +52476,3099 @@
       <c r="AMI31" s="0"/>
       <c r="AMJ31" s="0"/>
     </row>
-    <row r="38" s="129" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="130"/>
-      <c r="D38" s="130"/>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0"/>
+      <c r="B32" s="135" t="n">
+        <v>3</v>
+      </c>
+      <c r="C32" s="135" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="135" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" s="0"/>
+      <c r="F32" s="0"/>
+      <c r="G32" s="0"/>
+      <c r="H32" s="0"/>
+      <c r="I32" s="0"/>
+      <c r="J32" s="0"/>
+      <c r="K32" s="0"/>
+      <c r="L32" s="0"/>
+      <c r="M32" s="0"/>
+      <c r="N32" s="0"/>
+      <c r="O32" s="0"/>
+      <c r="P32" s="0"/>
+      <c r="Q32" s="0"/>
+      <c r="R32" s="0"/>
+      <c r="S32" s="0"/>
+      <c r="T32" s="0"/>
+      <c r="U32" s="0"/>
+      <c r="V32" s="0"/>
+      <c r="W32" s="0"/>
+      <c r="X32" s="0"/>
+      <c r="Y32" s="0"/>
+      <c r="Z32" s="0"/>
+      <c r="AA32" s="0"/>
+      <c r="AB32" s="0"/>
+      <c r="AC32" s="0"/>
+      <c r="AD32" s="0"/>
+      <c r="AE32" s="0"/>
+      <c r="AF32" s="0"/>
+      <c r="AG32" s="0"/>
+      <c r="AH32" s="0"/>
+      <c r="AI32" s="0"/>
+      <c r="AJ32" s="0"/>
+      <c r="AK32" s="0"/>
+      <c r="AL32" s="0"/>
+      <c r="AM32" s="0"/>
+      <c r="AN32" s="0"/>
+      <c r="AO32" s="0"/>
+      <c r="AP32" s="0"/>
+      <c r="AQ32" s="0"/>
+      <c r="AR32" s="0"/>
+      <c r="AS32" s="0"/>
+      <c r="AT32" s="0"/>
+      <c r="AU32" s="0"/>
+      <c r="AV32" s="0"/>
+      <c r="AW32" s="0"/>
+      <c r="AX32" s="0"/>
+      <c r="AY32" s="0"/>
+      <c r="AZ32" s="0"/>
+      <c r="BA32" s="0"/>
+      <c r="BB32" s="0"/>
+      <c r="BC32" s="0"/>
+      <c r="BD32" s="0"/>
+      <c r="BE32" s="0"/>
+      <c r="BF32" s="0"/>
+      <c r="BG32" s="0"/>
+      <c r="BH32" s="0"/>
+      <c r="BI32" s="0"/>
+      <c r="BJ32" s="0"/>
+      <c r="BK32" s="0"/>
+      <c r="BL32" s="0"/>
+      <c r="BM32" s="0"/>
+      <c r="BN32" s="0"/>
+      <c r="BO32" s="0"/>
+      <c r="BP32" s="0"/>
+      <c r="BQ32" s="0"/>
+      <c r="BR32" s="0"/>
+      <c r="BS32" s="0"/>
+      <c r="BT32" s="0"/>
+      <c r="BU32" s="0"/>
+      <c r="BV32" s="0"/>
+      <c r="BW32" s="0"/>
+      <c r="BX32" s="0"/>
+      <c r="BY32" s="0"/>
+      <c r="BZ32" s="0"/>
+      <c r="CA32" s="0"/>
+      <c r="CB32" s="0"/>
+      <c r="CC32" s="0"/>
+      <c r="CD32" s="0"/>
+      <c r="CE32" s="0"/>
+      <c r="CF32" s="0"/>
+      <c r="CG32" s="0"/>
+      <c r="CH32" s="0"/>
+      <c r="CI32" s="0"/>
+      <c r="CJ32" s="0"/>
+      <c r="CK32" s="0"/>
+      <c r="CL32" s="0"/>
+      <c r="CM32" s="0"/>
+      <c r="CN32" s="0"/>
+      <c r="CO32" s="0"/>
+      <c r="CP32" s="0"/>
+      <c r="CQ32" s="0"/>
+      <c r="CR32" s="0"/>
+      <c r="CS32" s="0"/>
+      <c r="CT32" s="0"/>
+      <c r="CU32" s="0"/>
+      <c r="CV32" s="0"/>
+      <c r="CW32" s="0"/>
+      <c r="CX32" s="0"/>
+      <c r="CY32" s="0"/>
+      <c r="CZ32" s="0"/>
+      <c r="DA32" s="0"/>
+      <c r="DB32" s="0"/>
+      <c r="DC32" s="0"/>
+      <c r="DD32" s="0"/>
+      <c r="DE32" s="0"/>
+      <c r="DF32" s="0"/>
+      <c r="DG32" s="0"/>
+      <c r="DH32" s="0"/>
+      <c r="DI32" s="0"/>
+      <c r="DJ32" s="0"/>
+      <c r="DK32" s="0"/>
+      <c r="DL32" s="0"/>
+      <c r="DM32" s="0"/>
+      <c r="DN32" s="0"/>
+      <c r="DO32" s="0"/>
+      <c r="DP32" s="0"/>
+      <c r="DQ32" s="0"/>
+      <c r="DR32" s="0"/>
+      <c r="DS32" s="0"/>
+      <c r="DT32" s="0"/>
+      <c r="DU32" s="0"/>
+      <c r="DV32" s="0"/>
+      <c r="DW32" s="0"/>
+      <c r="DX32" s="0"/>
+      <c r="DY32" s="0"/>
+      <c r="DZ32" s="0"/>
+      <c r="EA32" s="0"/>
+      <c r="EB32" s="0"/>
+      <c r="EC32" s="0"/>
+      <c r="ED32" s="0"/>
+      <c r="EE32" s="0"/>
+      <c r="EF32" s="0"/>
+      <c r="EG32" s="0"/>
+      <c r="EH32" s="0"/>
+      <c r="EI32" s="0"/>
+      <c r="EJ32" s="0"/>
+      <c r="EK32" s="0"/>
+      <c r="EL32" s="0"/>
+      <c r="EM32" s="0"/>
+      <c r="EN32" s="0"/>
+      <c r="EO32" s="0"/>
+      <c r="EP32" s="0"/>
+      <c r="EQ32" s="0"/>
+      <c r="ER32" s="0"/>
+      <c r="ES32" s="0"/>
+      <c r="ET32" s="0"/>
+      <c r="EU32" s="0"/>
+      <c r="EV32" s="0"/>
+      <c r="EW32" s="0"/>
+      <c r="EX32" s="0"/>
+      <c r="EY32" s="0"/>
+      <c r="EZ32" s="0"/>
+      <c r="FA32" s="0"/>
+      <c r="FB32" s="0"/>
+      <c r="FC32" s="0"/>
+      <c r="FD32" s="0"/>
+      <c r="FE32" s="0"/>
+      <c r="FF32" s="0"/>
+      <c r="FG32" s="0"/>
+      <c r="FH32" s="0"/>
+      <c r="FI32" s="0"/>
+      <c r="FJ32" s="0"/>
+      <c r="FK32" s="0"/>
+      <c r="FL32" s="0"/>
+      <c r="FM32" s="0"/>
+      <c r="FN32" s="0"/>
+      <c r="FO32" s="0"/>
+      <c r="FP32" s="0"/>
+      <c r="FQ32" s="0"/>
+      <c r="FR32" s="0"/>
+      <c r="FS32" s="0"/>
+      <c r="FT32" s="0"/>
+      <c r="FU32" s="0"/>
+      <c r="FV32" s="0"/>
+      <c r="FW32" s="0"/>
+      <c r="FX32" s="0"/>
+      <c r="FY32" s="0"/>
+      <c r="FZ32" s="0"/>
+      <c r="GA32" s="0"/>
+      <c r="GB32" s="0"/>
+      <c r="GC32" s="0"/>
+      <c r="GD32" s="0"/>
+      <c r="GE32" s="0"/>
+      <c r="GF32" s="0"/>
+      <c r="GG32" s="0"/>
+      <c r="GH32" s="0"/>
+      <c r="GI32" s="0"/>
+      <c r="GJ32" s="0"/>
+      <c r="GK32" s="0"/>
+      <c r="GL32" s="0"/>
+      <c r="GM32" s="0"/>
+      <c r="GN32" s="0"/>
+      <c r="GO32" s="0"/>
+      <c r="GP32" s="0"/>
+      <c r="GQ32" s="0"/>
+      <c r="GR32" s="0"/>
+      <c r="GS32" s="0"/>
+      <c r="GT32" s="0"/>
+      <c r="GU32" s="0"/>
+      <c r="GV32" s="0"/>
+      <c r="GW32" s="0"/>
+      <c r="GX32" s="0"/>
+      <c r="GY32" s="0"/>
+      <c r="GZ32" s="0"/>
+      <c r="HA32" s="0"/>
+      <c r="HB32" s="0"/>
+      <c r="HC32" s="0"/>
+      <c r="HD32" s="0"/>
+      <c r="HE32" s="0"/>
+      <c r="HF32" s="0"/>
+      <c r="HG32" s="0"/>
+      <c r="HH32" s="0"/>
+      <c r="HI32" s="0"/>
+      <c r="HJ32" s="0"/>
+      <c r="HK32" s="0"/>
+      <c r="HL32" s="0"/>
+      <c r="HM32" s="0"/>
+      <c r="HN32" s="0"/>
+      <c r="HO32" s="0"/>
+      <c r="HP32" s="0"/>
+      <c r="HQ32" s="0"/>
+      <c r="HR32" s="0"/>
+      <c r="HS32" s="0"/>
+      <c r="HT32" s="0"/>
+      <c r="HU32" s="0"/>
+      <c r="HV32" s="0"/>
+      <c r="HW32" s="0"/>
+      <c r="HX32" s="0"/>
+      <c r="HY32" s="0"/>
+      <c r="HZ32" s="0"/>
+      <c r="IA32" s="0"/>
+      <c r="IB32" s="0"/>
+      <c r="IC32" s="0"/>
+      <c r="ID32" s="0"/>
+      <c r="IE32" s="0"/>
+      <c r="IF32" s="0"/>
+      <c r="IG32" s="0"/>
+      <c r="IH32" s="0"/>
+      <c r="II32" s="0"/>
+      <c r="IJ32" s="0"/>
+      <c r="IK32" s="0"/>
+      <c r="IL32" s="0"/>
+      <c r="IM32" s="0"/>
+      <c r="IN32" s="0"/>
+      <c r="IO32" s="0"/>
+      <c r="IP32" s="0"/>
+      <c r="IQ32" s="0"/>
+      <c r="IR32" s="0"/>
+      <c r="IS32" s="0"/>
+      <c r="IT32" s="0"/>
+      <c r="IU32" s="0"/>
+      <c r="IV32" s="0"/>
+      <c r="IW32" s="0"/>
+      <c r="IX32" s="0"/>
+      <c r="IY32" s="0"/>
+      <c r="IZ32" s="0"/>
+      <c r="JA32" s="0"/>
+      <c r="JB32" s="0"/>
+      <c r="JC32" s="0"/>
+      <c r="JD32" s="0"/>
+      <c r="JE32" s="0"/>
+      <c r="JF32" s="0"/>
+      <c r="JG32" s="0"/>
+      <c r="JH32" s="0"/>
+      <c r="JI32" s="0"/>
+      <c r="JJ32" s="0"/>
+      <c r="JK32" s="0"/>
+      <c r="JL32" s="0"/>
+      <c r="JM32" s="0"/>
+      <c r="JN32" s="0"/>
+      <c r="JO32" s="0"/>
+      <c r="JP32" s="0"/>
+      <c r="JQ32" s="0"/>
+      <c r="JR32" s="0"/>
+      <c r="JS32" s="0"/>
+      <c r="JT32" s="0"/>
+      <c r="JU32" s="0"/>
+      <c r="JV32" s="0"/>
+      <c r="JW32" s="0"/>
+      <c r="JX32" s="0"/>
+      <c r="JY32" s="0"/>
+      <c r="JZ32" s="0"/>
+      <c r="KA32" s="0"/>
+      <c r="KB32" s="0"/>
+      <c r="KC32" s="0"/>
+      <c r="KD32" s="0"/>
+      <c r="KE32" s="0"/>
+      <c r="KF32" s="0"/>
+      <c r="KG32" s="0"/>
+      <c r="KH32" s="0"/>
+      <c r="KI32" s="0"/>
+      <c r="KJ32" s="0"/>
+      <c r="KK32" s="0"/>
+      <c r="KL32" s="0"/>
+      <c r="KM32" s="0"/>
+      <c r="KN32" s="0"/>
+      <c r="KO32" s="0"/>
+      <c r="KP32" s="0"/>
+      <c r="KQ32" s="0"/>
+      <c r="KR32" s="0"/>
+      <c r="KS32" s="0"/>
+      <c r="KT32" s="0"/>
+      <c r="KU32" s="0"/>
+      <c r="KV32" s="0"/>
+      <c r="KW32" s="0"/>
+      <c r="KX32" s="0"/>
+      <c r="KY32" s="0"/>
+      <c r="KZ32" s="0"/>
+      <c r="LA32" s="0"/>
+      <c r="LB32" s="0"/>
+      <c r="LC32" s="0"/>
+      <c r="LD32" s="0"/>
+      <c r="LE32" s="0"/>
+      <c r="LF32" s="0"/>
+      <c r="LG32" s="0"/>
+      <c r="LH32" s="0"/>
+      <c r="LI32" s="0"/>
+      <c r="LJ32" s="0"/>
+      <c r="LK32" s="0"/>
+      <c r="LL32" s="0"/>
+      <c r="LM32" s="0"/>
+      <c r="LN32" s="0"/>
+      <c r="LO32" s="0"/>
+      <c r="LP32" s="0"/>
+      <c r="LQ32" s="0"/>
+      <c r="LR32" s="0"/>
+      <c r="LS32" s="0"/>
+      <c r="LT32" s="0"/>
+      <c r="LU32" s="0"/>
+      <c r="LV32" s="0"/>
+      <c r="LW32" s="0"/>
+      <c r="LX32" s="0"/>
+      <c r="LY32" s="0"/>
+      <c r="LZ32" s="0"/>
+      <c r="MA32" s="0"/>
+      <c r="MB32" s="0"/>
+      <c r="MC32" s="0"/>
+      <c r="MD32" s="0"/>
+      <c r="ME32" s="0"/>
+      <c r="MF32" s="0"/>
+      <c r="MG32" s="0"/>
+      <c r="MH32" s="0"/>
+      <c r="MI32" s="0"/>
+      <c r="MJ32" s="0"/>
+      <c r="MK32" s="0"/>
+      <c r="ML32" s="0"/>
+      <c r="MM32" s="0"/>
+      <c r="MN32" s="0"/>
+      <c r="MO32" s="0"/>
+      <c r="MP32" s="0"/>
+      <c r="MQ32" s="0"/>
+      <c r="MR32" s="0"/>
+      <c r="MS32" s="0"/>
+      <c r="MT32" s="0"/>
+      <c r="MU32" s="0"/>
+      <c r="MV32" s="0"/>
+      <c r="MW32" s="0"/>
+      <c r="MX32" s="0"/>
+      <c r="MY32" s="0"/>
+      <c r="MZ32" s="0"/>
+      <c r="NA32" s="0"/>
+      <c r="NB32" s="0"/>
+      <c r="NC32" s="0"/>
+      <c r="ND32" s="0"/>
+      <c r="NE32" s="0"/>
+      <c r="NF32" s="0"/>
+      <c r="NG32" s="0"/>
+      <c r="NH32" s="0"/>
+      <c r="NI32" s="0"/>
+      <c r="NJ32" s="0"/>
+      <c r="NK32" s="0"/>
+      <c r="NL32" s="0"/>
+      <c r="NM32" s="0"/>
+      <c r="NN32" s="0"/>
+      <c r="NO32" s="0"/>
+      <c r="NP32" s="0"/>
+      <c r="NQ32" s="0"/>
+      <c r="NR32" s="0"/>
+      <c r="NS32" s="0"/>
+      <c r="NT32" s="0"/>
+      <c r="NU32" s="0"/>
+      <c r="NV32" s="0"/>
+      <c r="NW32" s="0"/>
+      <c r="NX32" s="0"/>
+      <c r="NY32" s="0"/>
+      <c r="NZ32" s="0"/>
+      <c r="OA32" s="0"/>
+      <c r="OB32" s="0"/>
+      <c r="OC32" s="0"/>
+      <c r="OD32" s="0"/>
+      <c r="OE32" s="0"/>
+      <c r="OF32" s="0"/>
+      <c r="OG32" s="0"/>
+      <c r="OH32" s="0"/>
+      <c r="OI32" s="0"/>
+      <c r="OJ32" s="0"/>
+      <c r="OK32" s="0"/>
+      <c r="OL32" s="0"/>
+      <c r="OM32" s="0"/>
+      <c r="ON32" s="0"/>
+      <c r="OO32" s="0"/>
+      <c r="OP32" s="0"/>
+      <c r="OQ32" s="0"/>
+      <c r="OR32" s="0"/>
+      <c r="OS32" s="0"/>
+      <c r="OT32" s="0"/>
+      <c r="OU32" s="0"/>
+      <c r="OV32" s="0"/>
+      <c r="OW32" s="0"/>
+      <c r="OX32" s="0"/>
+      <c r="OY32" s="0"/>
+      <c r="OZ32" s="0"/>
+      <c r="PA32" s="0"/>
+      <c r="PB32" s="0"/>
+      <c r="PC32" s="0"/>
+      <c r="PD32" s="0"/>
+      <c r="PE32" s="0"/>
+      <c r="PF32" s="0"/>
+      <c r="PG32" s="0"/>
+      <c r="PH32" s="0"/>
+      <c r="PI32" s="0"/>
+      <c r="PJ32" s="0"/>
+      <c r="PK32" s="0"/>
+      <c r="PL32" s="0"/>
+      <c r="PM32" s="0"/>
+      <c r="PN32" s="0"/>
+      <c r="PO32" s="0"/>
+      <c r="PP32" s="0"/>
+      <c r="PQ32" s="0"/>
+      <c r="PR32" s="0"/>
+      <c r="PS32" s="0"/>
+      <c r="PT32" s="0"/>
+      <c r="PU32" s="0"/>
+      <c r="PV32" s="0"/>
+      <c r="PW32" s="0"/>
+      <c r="PX32" s="0"/>
+      <c r="PY32" s="0"/>
+      <c r="PZ32" s="0"/>
+      <c r="QA32" s="0"/>
+      <c r="QB32" s="0"/>
+      <c r="QC32" s="0"/>
+      <c r="QD32" s="0"/>
+      <c r="QE32" s="0"/>
+      <c r="QF32" s="0"/>
+      <c r="QG32" s="0"/>
+      <c r="QH32" s="0"/>
+      <c r="QI32" s="0"/>
+      <c r="QJ32" s="0"/>
+      <c r="QK32" s="0"/>
+      <c r="QL32" s="0"/>
+      <c r="QM32" s="0"/>
+      <c r="QN32" s="0"/>
+      <c r="QO32" s="0"/>
+      <c r="QP32" s="0"/>
+      <c r="QQ32" s="0"/>
+      <c r="QR32" s="0"/>
+      <c r="QS32" s="0"/>
+      <c r="QT32" s="0"/>
+      <c r="QU32" s="0"/>
+      <c r="QV32" s="0"/>
+      <c r="QW32" s="0"/>
+      <c r="QX32" s="0"/>
+      <c r="QY32" s="0"/>
+      <c r="QZ32" s="0"/>
+      <c r="RA32" s="0"/>
+      <c r="RB32" s="0"/>
+      <c r="RC32" s="0"/>
+      <c r="RD32" s="0"/>
+      <c r="RE32" s="0"/>
+      <c r="RF32" s="0"/>
+      <c r="RG32" s="0"/>
+      <c r="RH32" s="0"/>
+      <c r="RI32" s="0"/>
+      <c r="RJ32" s="0"/>
+      <c r="RK32" s="0"/>
+      <c r="RL32" s="0"/>
+      <c r="RM32" s="0"/>
+      <c r="RN32" s="0"/>
+      <c r="RO32" s="0"/>
+      <c r="RP32" s="0"/>
+      <c r="RQ32" s="0"/>
+      <c r="RR32" s="0"/>
+      <c r="RS32" s="0"/>
+      <c r="RT32" s="0"/>
+      <c r="RU32" s="0"/>
+      <c r="RV32" s="0"/>
+      <c r="RW32" s="0"/>
+      <c r="RX32" s="0"/>
+      <c r="RY32" s="0"/>
+      <c r="RZ32" s="0"/>
+      <c r="SA32" s="0"/>
+      <c r="SB32" s="0"/>
+      <c r="SC32" s="0"/>
+      <c r="SD32" s="0"/>
+      <c r="SE32" s="0"/>
+      <c r="SF32" s="0"/>
+      <c r="SG32" s="0"/>
+      <c r="SH32" s="0"/>
+      <c r="SI32" s="0"/>
+      <c r="SJ32" s="0"/>
+      <c r="SK32" s="0"/>
+      <c r="SL32" s="0"/>
+      <c r="SM32" s="0"/>
+      <c r="SN32" s="0"/>
+      <c r="SO32" s="0"/>
+      <c r="SP32" s="0"/>
+      <c r="SQ32" s="0"/>
+      <c r="SR32" s="0"/>
+      <c r="SS32" s="0"/>
+      <c r="ST32" s="0"/>
+      <c r="SU32" s="0"/>
+      <c r="SV32" s="0"/>
+      <c r="SW32" s="0"/>
+      <c r="SX32" s="0"/>
+      <c r="SY32" s="0"/>
+      <c r="SZ32" s="0"/>
+      <c r="TA32" s="0"/>
+      <c r="TB32" s="0"/>
+      <c r="TC32" s="0"/>
+      <c r="TD32" s="0"/>
+      <c r="TE32" s="0"/>
+      <c r="TF32" s="0"/>
+      <c r="TG32" s="0"/>
+      <c r="TH32" s="0"/>
+      <c r="TI32" s="0"/>
+      <c r="TJ32" s="0"/>
+      <c r="TK32" s="0"/>
+      <c r="TL32" s="0"/>
+      <c r="TM32" s="0"/>
+      <c r="TN32" s="0"/>
+      <c r="TO32" s="0"/>
+      <c r="TP32" s="0"/>
+      <c r="TQ32" s="0"/>
+      <c r="TR32" s="0"/>
+      <c r="TS32" s="0"/>
+      <c r="TT32" s="0"/>
+      <c r="TU32" s="0"/>
+      <c r="TV32" s="0"/>
+      <c r="TW32" s="0"/>
+      <c r="TX32" s="0"/>
+      <c r="TY32" s="0"/>
+      <c r="TZ32" s="0"/>
+      <c r="UA32" s="0"/>
+      <c r="UB32" s="0"/>
+      <c r="UC32" s="0"/>
+      <c r="UD32" s="0"/>
+      <c r="UE32" s="0"/>
+      <c r="UF32" s="0"/>
+      <c r="UG32" s="0"/>
+      <c r="UH32" s="0"/>
+      <c r="UI32" s="0"/>
+      <c r="UJ32" s="0"/>
+      <c r="UK32" s="0"/>
+      <c r="UL32" s="0"/>
+      <c r="UM32" s="0"/>
+      <c r="UN32" s="0"/>
+      <c r="UO32" s="0"/>
+      <c r="UP32" s="0"/>
+      <c r="UQ32" s="0"/>
+      <c r="UR32" s="0"/>
+      <c r="US32" s="0"/>
+      <c r="UT32" s="0"/>
+      <c r="UU32" s="0"/>
+      <c r="UV32" s="0"/>
+      <c r="UW32" s="0"/>
+      <c r="UX32" s="0"/>
+      <c r="UY32" s="0"/>
+      <c r="UZ32" s="0"/>
+      <c r="VA32" s="0"/>
+      <c r="VB32" s="0"/>
+      <c r="VC32" s="0"/>
+      <c r="VD32" s="0"/>
+      <c r="VE32" s="0"/>
+      <c r="VF32" s="0"/>
+      <c r="VG32" s="0"/>
+      <c r="VH32" s="0"/>
+      <c r="VI32" s="0"/>
+      <c r="VJ32" s="0"/>
+      <c r="VK32" s="0"/>
+      <c r="VL32" s="0"/>
+      <c r="VM32" s="0"/>
+      <c r="VN32" s="0"/>
+      <c r="VO32" s="0"/>
+      <c r="VP32" s="0"/>
+      <c r="VQ32" s="0"/>
+      <c r="VR32" s="0"/>
+      <c r="VS32" s="0"/>
+      <c r="VT32" s="0"/>
+      <c r="VU32" s="0"/>
+      <c r="VV32" s="0"/>
+      <c r="VW32" s="0"/>
+      <c r="VX32" s="0"/>
+      <c r="VY32" s="0"/>
+      <c r="VZ32" s="0"/>
+      <c r="WA32" s="0"/>
+      <c r="WB32" s="0"/>
+      <c r="WC32" s="0"/>
+      <c r="WD32" s="0"/>
+      <c r="WE32" s="0"/>
+      <c r="WF32" s="0"/>
+      <c r="WG32" s="0"/>
+      <c r="WH32" s="0"/>
+      <c r="WI32" s="0"/>
+      <c r="WJ32" s="0"/>
+      <c r="WK32" s="0"/>
+      <c r="WL32" s="0"/>
+      <c r="WM32" s="0"/>
+      <c r="WN32" s="0"/>
+      <c r="WO32" s="0"/>
+      <c r="WP32" s="0"/>
+      <c r="WQ32" s="0"/>
+      <c r="WR32" s="0"/>
+      <c r="WS32" s="0"/>
+      <c r="WT32" s="0"/>
+      <c r="WU32" s="0"/>
+      <c r="WV32" s="0"/>
+      <c r="WW32" s="0"/>
+      <c r="WX32" s="0"/>
+      <c r="WY32" s="0"/>
+      <c r="WZ32" s="0"/>
+      <c r="XA32" s="0"/>
+      <c r="XB32" s="0"/>
+      <c r="XC32" s="0"/>
+      <c r="XD32" s="0"/>
+      <c r="XE32" s="0"/>
+      <c r="XF32" s="0"/>
+      <c r="XG32" s="0"/>
+      <c r="XH32" s="0"/>
+      <c r="XI32" s="0"/>
+      <c r="XJ32" s="0"/>
+      <c r="XK32" s="0"/>
+      <c r="XL32" s="0"/>
+      <c r="XM32" s="0"/>
+      <c r="XN32" s="0"/>
+      <c r="XO32" s="0"/>
+      <c r="XP32" s="0"/>
+      <c r="XQ32" s="0"/>
+      <c r="XR32" s="0"/>
+      <c r="XS32" s="0"/>
+      <c r="XT32" s="0"/>
+      <c r="XU32" s="0"/>
+      <c r="XV32" s="0"/>
+      <c r="XW32" s="0"/>
+      <c r="XX32" s="0"/>
+      <c r="XY32" s="0"/>
+      <c r="XZ32" s="0"/>
+      <c r="YA32" s="0"/>
+      <c r="YB32" s="0"/>
+      <c r="YC32" s="0"/>
+      <c r="YD32" s="0"/>
+      <c r="YE32" s="0"/>
+      <c r="YF32" s="0"/>
+      <c r="YG32" s="0"/>
+      <c r="YH32" s="0"/>
+      <c r="YI32" s="0"/>
+      <c r="YJ32" s="0"/>
+      <c r="YK32" s="0"/>
+      <c r="YL32" s="0"/>
+      <c r="YM32" s="0"/>
+      <c r="YN32" s="0"/>
+      <c r="YO32" s="0"/>
+      <c r="YP32" s="0"/>
+      <c r="YQ32" s="0"/>
+      <c r="YR32" s="0"/>
+      <c r="YS32" s="0"/>
+      <c r="YT32" s="0"/>
+      <c r="YU32" s="0"/>
+      <c r="YV32" s="0"/>
+      <c r="YW32" s="0"/>
+      <c r="YX32" s="0"/>
+      <c r="YY32" s="0"/>
+      <c r="YZ32" s="0"/>
+      <c r="ZA32" s="0"/>
+      <c r="ZB32" s="0"/>
+      <c r="ZC32" s="0"/>
+      <c r="ZD32" s="0"/>
+      <c r="ZE32" s="0"/>
+      <c r="ZF32" s="0"/>
+      <c r="ZG32" s="0"/>
+      <c r="ZH32" s="0"/>
+      <c r="ZI32" s="0"/>
+      <c r="ZJ32" s="0"/>
+      <c r="ZK32" s="0"/>
+      <c r="ZL32" s="0"/>
+      <c r="ZM32" s="0"/>
+      <c r="ZN32" s="0"/>
+      <c r="ZO32" s="0"/>
+      <c r="ZP32" s="0"/>
+      <c r="ZQ32" s="0"/>
+      <c r="ZR32" s="0"/>
+      <c r="ZS32" s="0"/>
+      <c r="ZT32" s="0"/>
+      <c r="ZU32" s="0"/>
+      <c r="ZV32" s="0"/>
+      <c r="ZW32" s="0"/>
+      <c r="ZX32" s="0"/>
+      <c r="ZY32" s="0"/>
+      <c r="ZZ32" s="0"/>
+      <c r="AAA32" s="0"/>
+      <c r="AAB32" s="0"/>
+      <c r="AAC32" s="0"/>
+      <c r="AAD32" s="0"/>
+      <c r="AAE32" s="0"/>
+      <c r="AAF32" s="0"/>
+      <c r="AAG32" s="0"/>
+      <c r="AAH32" s="0"/>
+      <c r="AAI32" s="0"/>
+      <c r="AAJ32" s="0"/>
+      <c r="AAK32" s="0"/>
+      <c r="AAL32" s="0"/>
+      <c r="AAM32" s="0"/>
+      <c r="AAN32" s="0"/>
+      <c r="AAO32" s="0"/>
+      <c r="AAP32" s="0"/>
+      <c r="AAQ32" s="0"/>
+      <c r="AAR32" s="0"/>
+      <c r="AAS32" s="0"/>
+      <c r="AAT32" s="0"/>
+      <c r="AAU32" s="0"/>
+      <c r="AAV32" s="0"/>
+      <c r="AAW32" s="0"/>
+      <c r="AAX32" s="0"/>
+      <c r="AAY32" s="0"/>
+      <c r="AAZ32" s="0"/>
+      <c r="ABA32" s="0"/>
+      <c r="ABB32" s="0"/>
+      <c r="ABC32" s="0"/>
+      <c r="ABD32" s="0"/>
+      <c r="ABE32" s="0"/>
+      <c r="ABF32" s="0"/>
+      <c r="ABG32" s="0"/>
+      <c r="ABH32" s="0"/>
+      <c r="ABI32" s="0"/>
+      <c r="ABJ32" s="0"/>
+      <c r="ABK32" s="0"/>
+      <c r="ABL32" s="0"/>
+      <c r="ABM32" s="0"/>
+      <c r="ABN32" s="0"/>
+      <c r="ABO32" s="0"/>
+      <c r="ABP32" s="0"/>
+      <c r="ABQ32" s="0"/>
+      <c r="ABR32" s="0"/>
+      <c r="ABS32" s="0"/>
+      <c r="ABT32" s="0"/>
+      <c r="ABU32" s="0"/>
+      <c r="ABV32" s="0"/>
+      <c r="ABW32" s="0"/>
+      <c r="ABX32" s="0"/>
+      <c r="ABY32" s="0"/>
+      <c r="ABZ32" s="0"/>
+      <c r="ACA32" s="0"/>
+      <c r="ACB32" s="0"/>
+      <c r="ACC32" s="0"/>
+      <c r="ACD32" s="0"/>
+      <c r="ACE32" s="0"/>
+      <c r="ACF32" s="0"/>
+      <c r="ACG32" s="0"/>
+      <c r="ACH32" s="0"/>
+      <c r="ACI32" s="0"/>
+      <c r="ACJ32" s="0"/>
+      <c r="ACK32" s="0"/>
+      <c r="ACL32" s="0"/>
+      <c r="ACM32" s="0"/>
+      <c r="ACN32" s="0"/>
+      <c r="ACO32" s="0"/>
+      <c r="ACP32" s="0"/>
+      <c r="ACQ32" s="0"/>
+      <c r="ACR32" s="0"/>
+      <c r="ACS32" s="0"/>
+      <c r="ACT32" s="0"/>
+      <c r="ACU32" s="0"/>
+      <c r="ACV32" s="0"/>
+      <c r="ACW32" s="0"/>
+      <c r="ACX32" s="0"/>
+      <c r="ACY32" s="0"/>
+      <c r="ACZ32" s="0"/>
+      <c r="ADA32" s="0"/>
+      <c r="ADB32" s="0"/>
+      <c r="ADC32" s="0"/>
+      <c r="ADD32" s="0"/>
+      <c r="ADE32" s="0"/>
+      <c r="ADF32" s="0"/>
+      <c r="ADG32" s="0"/>
+      <c r="ADH32" s="0"/>
+      <c r="ADI32" s="0"/>
+      <c r="ADJ32" s="0"/>
+      <c r="ADK32" s="0"/>
+      <c r="ADL32" s="0"/>
+      <c r="ADM32" s="0"/>
+      <c r="ADN32" s="0"/>
+      <c r="ADO32" s="0"/>
+      <c r="ADP32" s="0"/>
+      <c r="ADQ32" s="0"/>
+      <c r="ADR32" s="0"/>
+      <c r="ADS32" s="0"/>
+      <c r="ADT32" s="0"/>
+      <c r="ADU32" s="0"/>
+      <c r="ADV32" s="0"/>
+      <c r="ADW32" s="0"/>
+      <c r="ADX32" s="0"/>
+      <c r="ADY32" s="0"/>
+      <c r="ADZ32" s="0"/>
+      <c r="AEA32" s="0"/>
+      <c r="AEB32" s="0"/>
+      <c r="AEC32" s="0"/>
+      <c r="AED32" s="0"/>
+      <c r="AEE32" s="0"/>
+      <c r="AEF32" s="0"/>
+      <c r="AEG32" s="0"/>
+      <c r="AEH32" s="0"/>
+      <c r="AEI32" s="0"/>
+      <c r="AEJ32" s="0"/>
+      <c r="AEK32" s="0"/>
+      <c r="AEL32" s="0"/>
+      <c r="AEM32" s="0"/>
+      <c r="AEN32" s="0"/>
+      <c r="AEO32" s="0"/>
+      <c r="AEP32" s="0"/>
+      <c r="AEQ32" s="0"/>
+      <c r="AER32" s="0"/>
+      <c r="AES32" s="0"/>
+      <c r="AET32" s="0"/>
+      <c r="AEU32" s="0"/>
+      <c r="AEV32" s="0"/>
+      <c r="AEW32" s="0"/>
+      <c r="AEX32" s="0"/>
+      <c r="AEY32" s="0"/>
+      <c r="AEZ32" s="0"/>
+      <c r="AFA32" s="0"/>
+      <c r="AFB32" s="0"/>
+      <c r="AFC32" s="0"/>
+      <c r="AFD32" s="0"/>
+      <c r="AFE32" s="0"/>
+      <c r="AFF32" s="0"/>
+      <c r="AFG32" s="0"/>
+      <c r="AFH32" s="0"/>
+      <c r="AFI32" s="0"/>
+      <c r="AFJ32" s="0"/>
+      <c r="AFK32" s="0"/>
+      <c r="AFL32" s="0"/>
+      <c r="AFM32" s="0"/>
+      <c r="AFN32" s="0"/>
+      <c r="AFO32" s="0"/>
+      <c r="AFP32" s="0"/>
+      <c r="AFQ32" s="0"/>
+      <c r="AFR32" s="0"/>
+      <c r="AFS32" s="0"/>
+      <c r="AFT32" s="0"/>
+      <c r="AFU32" s="0"/>
+      <c r="AFV32" s="0"/>
+      <c r="AFW32" s="0"/>
+      <c r="AFX32" s="0"/>
+      <c r="AFY32" s="0"/>
+      <c r="AFZ32" s="0"/>
+      <c r="AGA32" s="0"/>
+      <c r="AGB32" s="0"/>
+      <c r="AGC32" s="0"/>
+      <c r="AGD32" s="0"/>
+      <c r="AGE32" s="0"/>
+      <c r="AGF32" s="0"/>
+      <c r="AGG32" s="0"/>
+      <c r="AGH32" s="0"/>
+      <c r="AGI32" s="0"/>
+      <c r="AGJ32" s="0"/>
+      <c r="AGK32" s="0"/>
+      <c r="AGL32" s="0"/>
+      <c r="AGM32" s="0"/>
+      <c r="AGN32" s="0"/>
+      <c r="AGO32" s="0"/>
+      <c r="AGP32" s="0"/>
+      <c r="AGQ32" s="0"/>
+      <c r="AGR32" s="0"/>
+      <c r="AGS32" s="0"/>
+      <c r="AGT32" s="0"/>
+      <c r="AGU32" s="0"/>
+      <c r="AGV32" s="0"/>
+      <c r="AGW32" s="0"/>
+      <c r="AGX32" s="0"/>
+      <c r="AGY32" s="0"/>
+      <c r="AGZ32" s="0"/>
+      <c r="AHA32" s="0"/>
+      <c r="AHB32" s="0"/>
+      <c r="AHC32" s="0"/>
+      <c r="AHD32" s="0"/>
+      <c r="AHE32" s="0"/>
+      <c r="AHF32" s="0"/>
+      <c r="AHG32" s="0"/>
+      <c r="AHH32" s="0"/>
+      <c r="AHI32" s="0"/>
+      <c r="AHJ32" s="0"/>
+      <c r="AHK32" s="0"/>
+      <c r="AHL32" s="0"/>
+      <c r="AHM32" s="0"/>
+      <c r="AHN32" s="0"/>
+      <c r="AHO32" s="0"/>
+      <c r="AHP32" s="0"/>
+      <c r="AHQ32" s="0"/>
+      <c r="AHR32" s="0"/>
+      <c r="AHS32" s="0"/>
+      <c r="AHT32" s="0"/>
+      <c r="AHU32" s="0"/>
+      <c r="AHV32" s="0"/>
+      <c r="AHW32" s="0"/>
+      <c r="AHX32" s="0"/>
+      <c r="AHY32" s="0"/>
+      <c r="AHZ32" s="0"/>
+      <c r="AIA32" s="0"/>
+      <c r="AIB32" s="0"/>
+      <c r="AIC32" s="0"/>
+      <c r="AID32" s="0"/>
+      <c r="AIE32" s="0"/>
+      <c r="AIF32" s="0"/>
+      <c r="AIG32" s="0"/>
+      <c r="AIH32" s="0"/>
+      <c r="AII32" s="0"/>
+      <c r="AIJ32" s="0"/>
+      <c r="AIK32" s="0"/>
+      <c r="AIL32" s="0"/>
+      <c r="AIM32" s="0"/>
+      <c r="AIN32" s="0"/>
+      <c r="AIO32" s="0"/>
+      <c r="AIP32" s="0"/>
+      <c r="AIQ32" s="0"/>
+      <c r="AIR32" s="0"/>
+      <c r="AIS32" s="0"/>
+      <c r="AIT32" s="0"/>
+      <c r="AIU32" s="0"/>
+      <c r="AIV32" s="0"/>
+      <c r="AIW32" s="0"/>
+      <c r="AIX32" s="0"/>
+      <c r="AIY32" s="0"/>
+      <c r="AIZ32" s="0"/>
+      <c r="AJA32" s="0"/>
+      <c r="AJB32" s="0"/>
+      <c r="AJC32" s="0"/>
+      <c r="AJD32" s="0"/>
+      <c r="AJE32" s="0"/>
+      <c r="AJF32" s="0"/>
+      <c r="AJG32" s="0"/>
+      <c r="AJH32" s="0"/>
+      <c r="AJI32" s="0"/>
+      <c r="AJJ32" s="0"/>
+      <c r="AJK32" s="0"/>
+      <c r="AJL32" s="0"/>
+      <c r="AJM32" s="0"/>
+      <c r="AJN32" s="0"/>
+      <c r="AJO32" s="0"/>
+      <c r="AJP32" s="0"/>
+      <c r="AJQ32" s="0"/>
+      <c r="AJR32" s="0"/>
+      <c r="AJS32" s="0"/>
+      <c r="AJT32" s="0"/>
+      <c r="AJU32" s="0"/>
+      <c r="AJV32" s="0"/>
+      <c r="AJW32" s="0"/>
+      <c r="AJX32" s="0"/>
+      <c r="AJY32" s="0"/>
+      <c r="AJZ32" s="0"/>
+      <c r="AKA32" s="0"/>
+      <c r="AKB32" s="0"/>
+      <c r="AKC32" s="0"/>
+      <c r="AKD32" s="0"/>
+      <c r="AKE32" s="0"/>
+      <c r="AKF32" s="0"/>
+      <c r="AKG32" s="0"/>
+      <c r="AKH32" s="0"/>
+      <c r="AKI32" s="0"/>
+      <c r="AKJ32" s="0"/>
+      <c r="AKK32" s="0"/>
+      <c r="AKL32" s="0"/>
+      <c r="AKM32" s="0"/>
+      <c r="AKN32" s="0"/>
+      <c r="AKO32" s="0"/>
+      <c r="AKP32" s="0"/>
+      <c r="AKQ32" s="0"/>
+      <c r="AKR32" s="0"/>
+      <c r="AKS32" s="0"/>
+      <c r="AKT32" s="0"/>
+      <c r="AKU32" s="0"/>
+      <c r="AKV32" s="0"/>
+      <c r="AKW32" s="0"/>
+      <c r="AKX32" s="0"/>
+      <c r="AKY32" s="0"/>
+      <c r="AKZ32" s="0"/>
+      <c r="ALA32" s="0"/>
+      <c r="ALB32" s="0"/>
+      <c r="ALC32" s="0"/>
+      <c r="ALD32" s="0"/>
+      <c r="ALE32" s="0"/>
+      <c r="ALF32" s="0"/>
+      <c r="ALG32" s="0"/>
+      <c r="ALH32" s="0"/>
+      <c r="ALI32" s="0"/>
+      <c r="ALJ32" s="0"/>
+      <c r="ALK32" s="0"/>
+      <c r="ALL32" s="0"/>
+      <c r="ALM32" s="0"/>
+      <c r="ALN32" s="0"/>
+      <c r="ALO32" s="0"/>
+      <c r="ALP32" s="0"/>
+      <c r="ALQ32" s="0"/>
+      <c r="ALR32" s="0"/>
+      <c r="ALS32" s="0"/>
+      <c r="ALT32" s="0"/>
+      <c r="ALU32" s="0"/>
+      <c r="ALV32" s="0"/>
+      <c r="ALW32" s="0"/>
+      <c r="ALX32" s="0"/>
+      <c r="ALY32" s="0"/>
+      <c r="ALZ32" s="0"/>
+      <c r="AMA32" s="0"/>
+      <c r="AMB32" s="0"/>
+      <c r="AMC32" s="0"/>
+      <c r="AMD32" s="0"/>
+      <c r="AME32" s="0"/>
+      <c r="AMF32" s="0"/>
+      <c r="AMG32" s="0"/>
+      <c r="AMH32" s="0"/>
+      <c r="AMI32" s="0"/>
+      <c r="AMJ32" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0"/>
+      <c r="B33" s="135" t="n">
+        <v>4</v>
+      </c>
+      <c r="C33" s="135" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" s="135" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" s="0"/>
+      <c r="F33" s="0"/>
+      <c r="G33" s="0"/>
+      <c r="H33" s="0"/>
+      <c r="I33" s="0"/>
+      <c r="J33" s="0"/>
+      <c r="K33" s="0"/>
+      <c r="L33" s="0"/>
+      <c r="M33" s="0"/>
+      <c r="N33" s="0"/>
+      <c r="O33" s="0"/>
+      <c r="P33" s="0"/>
+      <c r="Q33" s="0"/>
+      <c r="R33" s="0"/>
+      <c r="S33" s="0"/>
+      <c r="T33" s="0"/>
+      <c r="U33" s="0"/>
+      <c r="V33" s="0"/>
+      <c r="W33" s="0"/>
+      <c r="X33" s="0"/>
+      <c r="Y33" s="0"/>
+      <c r="Z33" s="0"/>
+      <c r="AA33" s="0"/>
+      <c r="AB33" s="0"/>
+      <c r="AC33" s="0"/>
+      <c r="AD33" s="0"/>
+      <c r="AE33" s="0"/>
+      <c r="AF33" s="0"/>
+      <c r="AG33" s="0"/>
+      <c r="AH33" s="0"/>
+      <c r="AI33" s="0"/>
+      <c r="AJ33" s="0"/>
+      <c r="AK33" s="0"/>
+      <c r="AL33" s="0"/>
+      <c r="AM33" s="0"/>
+      <c r="AN33" s="0"/>
+      <c r="AO33" s="0"/>
+      <c r="AP33" s="0"/>
+      <c r="AQ33" s="0"/>
+      <c r="AR33" s="0"/>
+      <c r="AS33" s="0"/>
+      <c r="AT33" s="0"/>
+      <c r="AU33" s="0"/>
+      <c r="AV33" s="0"/>
+      <c r="AW33" s="0"/>
+      <c r="AX33" s="0"/>
+      <c r="AY33" s="0"/>
+      <c r="AZ33" s="0"/>
+      <c r="BA33" s="0"/>
+      <c r="BB33" s="0"/>
+      <c r="BC33" s="0"/>
+      <c r="BD33" s="0"/>
+      <c r="BE33" s="0"/>
+      <c r="BF33" s="0"/>
+      <c r="BG33" s="0"/>
+      <c r="BH33" s="0"/>
+      <c r="BI33" s="0"/>
+      <c r="BJ33" s="0"/>
+      <c r="BK33" s="0"/>
+      <c r="BL33" s="0"/>
+      <c r="BM33" s="0"/>
+      <c r="BN33" s="0"/>
+      <c r="BO33" s="0"/>
+      <c r="BP33" s="0"/>
+      <c r="BQ33" s="0"/>
+      <c r="BR33" s="0"/>
+      <c r="BS33" s="0"/>
+      <c r="BT33" s="0"/>
+      <c r="BU33" s="0"/>
+      <c r="BV33" s="0"/>
+      <c r="BW33" s="0"/>
+      <c r="BX33" s="0"/>
+      <c r="BY33" s="0"/>
+      <c r="BZ33" s="0"/>
+      <c r="CA33" s="0"/>
+      <c r="CB33" s="0"/>
+      <c r="CC33" s="0"/>
+      <c r="CD33" s="0"/>
+      <c r="CE33" s="0"/>
+      <c r="CF33" s="0"/>
+      <c r="CG33" s="0"/>
+      <c r="CH33" s="0"/>
+      <c r="CI33" s="0"/>
+      <c r="CJ33" s="0"/>
+      <c r="CK33" s="0"/>
+      <c r="CL33" s="0"/>
+      <c r="CM33" s="0"/>
+      <c r="CN33" s="0"/>
+      <c r="CO33" s="0"/>
+      <c r="CP33" s="0"/>
+      <c r="CQ33" s="0"/>
+      <c r="CR33" s="0"/>
+      <c r="CS33" s="0"/>
+      <c r="CT33" s="0"/>
+      <c r="CU33" s="0"/>
+      <c r="CV33" s="0"/>
+      <c r="CW33" s="0"/>
+      <c r="CX33" s="0"/>
+      <c r="CY33" s="0"/>
+      <c r="CZ33" s="0"/>
+      <c r="DA33" s="0"/>
+      <c r="DB33" s="0"/>
+      <c r="DC33" s="0"/>
+      <c r="DD33" s="0"/>
+      <c r="DE33" s="0"/>
+      <c r="DF33" s="0"/>
+      <c r="DG33" s="0"/>
+      <c r="DH33" s="0"/>
+      <c r="DI33" s="0"/>
+      <c r="DJ33" s="0"/>
+      <c r="DK33" s="0"/>
+      <c r="DL33" s="0"/>
+      <c r="DM33" s="0"/>
+      <c r="DN33" s="0"/>
+      <c r="DO33" s="0"/>
+      <c r="DP33" s="0"/>
+      <c r="DQ33" s="0"/>
+      <c r="DR33" s="0"/>
+      <c r="DS33" s="0"/>
+      <c r="DT33" s="0"/>
+      <c r="DU33" s="0"/>
+      <c r="DV33" s="0"/>
+      <c r="DW33" s="0"/>
+      <c r="DX33" s="0"/>
+      <c r="DY33" s="0"/>
+      <c r="DZ33" s="0"/>
+      <c r="EA33" s="0"/>
+      <c r="EB33" s="0"/>
+      <c r="EC33" s="0"/>
+      <c r="ED33" s="0"/>
+      <c r="EE33" s="0"/>
+      <c r="EF33" s="0"/>
+      <c r="EG33" s="0"/>
+      <c r="EH33" s="0"/>
+      <c r="EI33" s="0"/>
+      <c r="EJ33" s="0"/>
+      <c r="EK33" s="0"/>
+      <c r="EL33" s="0"/>
+      <c r="EM33" s="0"/>
+      <c r="EN33" s="0"/>
+      <c r="EO33" s="0"/>
+      <c r="EP33" s="0"/>
+      <c r="EQ33" s="0"/>
+      <c r="ER33" s="0"/>
+      <c r="ES33" s="0"/>
+      <c r="ET33" s="0"/>
+      <c r="EU33" s="0"/>
+      <c r="EV33" s="0"/>
+      <c r="EW33" s="0"/>
+      <c r="EX33" s="0"/>
+      <c r="EY33" s="0"/>
+      <c r="EZ33" s="0"/>
+      <c r="FA33" s="0"/>
+      <c r="FB33" s="0"/>
+      <c r="FC33" s="0"/>
+      <c r="FD33" s="0"/>
+      <c r="FE33" s="0"/>
+      <c r="FF33" s="0"/>
+      <c r="FG33" s="0"/>
+      <c r="FH33" s="0"/>
+      <c r="FI33" s="0"/>
+      <c r="FJ33" s="0"/>
+      <c r="FK33" s="0"/>
+      <c r="FL33" s="0"/>
+      <c r="FM33" s="0"/>
+      <c r="FN33" s="0"/>
+      <c r="FO33" s="0"/>
+      <c r="FP33" s="0"/>
+      <c r="FQ33" s="0"/>
+      <c r="FR33" s="0"/>
+      <c r="FS33" s="0"/>
+      <c r="FT33" s="0"/>
+      <c r="FU33" s="0"/>
+      <c r="FV33" s="0"/>
+      <c r="FW33" s="0"/>
+      <c r="FX33" s="0"/>
+      <c r="FY33" s="0"/>
+      <c r="FZ33" s="0"/>
+      <c r="GA33" s="0"/>
+      <c r="GB33" s="0"/>
+      <c r="GC33" s="0"/>
+      <c r="GD33" s="0"/>
+      <c r="GE33" s="0"/>
+      <c r="GF33" s="0"/>
+      <c r="GG33" s="0"/>
+      <c r="GH33" s="0"/>
+      <c r="GI33" s="0"/>
+      <c r="GJ33" s="0"/>
+      <c r="GK33" s="0"/>
+      <c r="GL33" s="0"/>
+      <c r="GM33" s="0"/>
+      <c r="GN33" s="0"/>
+      <c r="GO33" s="0"/>
+      <c r="GP33" s="0"/>
+      <c r="GQ33" s="0"/>
+      <c r="GR33" s="0"/>
+      <c r="GS33" s="0"/>
+      <c r="GT33" s="0"/>
+      <c r="GU33" s="0"/>
+      <c r="GV33" s="0"/>
+      <c r="GW33" s="0"/>
+      <c r="GX33" s="0"/>
+      <c r="GY33" s="0"/>
+      <c r="GZ33" s="0"/>
+      <c r="HA33" s="0"/>
+      <c r="HB33" s="0"/>
+      <c r="HC33" s="0"/>
+      <c r="HD33" s="0"/>
+      <c r="HE33" s="0"/>
+      <c r="HF33" s="0"/>
+      <c r="HG33" s="0"/>
+      <c r="HH33" s="0"/>
+      <c r="HI33" s="0"/>
+      <c r="HJ33" s="0"/>
+      <c r="HK33" s="0"/>
+      <c r="HL33" s="0"/>
+      <c r="HM33" s="0"/>
+      <c r="HN33" s="0"/>
+      <c r="HO33" s="0"/>
+      <c r="HP33" s="0"/>
+      <c r="HQ33" s="0"/>
+      <c r="HR33" s="0"/>
+      <c r="HS33" s="0"/>
+      <c r="HT33" s="0"/>
+      <c r="HU33" s="0"/>
+      <c r="HV33" s="0"/>
+      <c r="HW33" s="0"/>
+      <c r="HX33" s="0"/>
+      <c r="HY33" s="0"/>
+      <c r="HZ33" s="0"/>
+      <c r="IA33" s="0"/>
+      <c r="IB33" s="0"/>
+      <c r="IC33" s="0"/>
+      <c r="ID33" s="0"/>
+      <c r="IE33" s="0"/>
+      <c r="IF33" s="0"/>
+      <c r="IG33" s="0"/>
+      <c r="IH33" s="0"/>
+      <c r="II33" s="0"/>
+      <c r="IJ33" s="0"/>
+      <c r="IK33" s="0"/>
+      <c r="IL33" s="0"/>
+      <c r="IM33" s="0"/>
+      <c r="IN33" s="0"/>
+      <c r="IO33" s="0"/>
+      <c r="IP33" s="0"/>
+      <c r="IQ33" s="0"/>
+      <c r="IR33" s="0"/>
+      <c r="IS33" s="0"/>
+      <c r="IT33" s="0"/>
+      <c r="IU33" s="0"/>
+      <c r="IV33" s="0"/>
+      <c r="IW33" s="0"/>
+      <c r="IX33" s="0"/>
+      <c r="IY33" s="0"/>
+      <c r="IZ33" s="0"/>
+      <c r="JA33" s="0"/>
+      <c r="JB33" s="0"/>
+      <c r="JC33" s="0"/>
+      <c r="JD33" s="0"/>
+      <c r="JE33" s="0"/>
+      <c r="JF33" s="0"/>
+      <c r="JG33" s="0"/>
+      <c r="JH33" s="0"/>
+      <c r="JI33" s="0"/>
+      <c r="JJ33" s="0"/>
+      <c r="JK33" s="0"/>
+      <c r="JL33" s="0"/>
+      <c r="JM33" s="0"/>
+      <c r="JN33" s="0"/>
+      <c r="JO33" s="0"/>
+      <c r="JP33" s="0"/>
+      <c r="JQ33" s="0"/>
+      <c r="JR33" s="0"/>
+      <c r="JS33" s="0"/>
+      <c r="JT33" s="0"/>
+      <c r="JU33" s="0"/>
+      <c r="JV33" s="0"/>
+      <c r="JW33" s="0"/>
+      <c r="JX33" s="0"/>
+      <c r="JY33" s="0"/>
+      <c r="JZ33" s="0"/>
+      <c r="KA33" s="0"/>
+      <c r="KB33" s="0"/>
+      <c r="KC33" s="0"/>
+      <c r="KD33" s="0"/>
+      <c r="KE33" s="0"/>
+      <c r="KF33" s="0"/>
+      <c r="KG33" s="0"/>
+      <c r="KH33" s="0"/>
+      <c r="KI33" s="0"/>
+      <c r="KJ33" s="0"/>
+      <c r="KK33" s="0"/>
+      <c r="KL33" s="0"/>
+      <c r="KM33" s="0"/>
+      <c r="KN33" s="0"/>
+      <c r="KO33" s="0"/>
+      <c r="KP33" s="0"/>
+      <c r="KQ33" s="0"/>
+      <c r="KR33" s="0"/>
+      <c r="KS33" s="0"/>
+      <c r="KT33" s="0"/>
+      <c r="KU33" s="0"/>
+      <c r="KV33" s="0"/>
+      <c r="KW33" s="0"/>
+      <c r="KX33" s="0"/>
+      <c r="KY33" s="0"/>
+      <c r="KZ33" s="0"/>
+      <c r="LA33" s="0"/>
+      <c r="LB33" s="0"/>
+      <c r="LC33" s="0"/>
+      <c r="LD33" s="0"/>
+      <c r="LE33" s="0"/>
+      <c r="LF33" s="0"/>
+      <c r="LG33" s="0"/>
+      <c r="LH33" s="0"/>
+      <c r="LI33" s="0"/>
+      <c r="LJ33" s="0"/>
+      <c r="LK33" s="0"/>
+      <c r="LL33" s="0"/>
+      <c r="LM33" s="0"/>
+      <c r="LN33" s="0"/>
+      <c r="LO33" s="0"/>
+      <c r="LP33" s="0"/>
+      <c r="LQ33" s="0"/>
+      <c r="LR33" s="0"/>
+      <c r="LS33" s="0"/>
+      <c r="LT33" s="0"/>
+      <c r="LU33" s="0"/>
+      <c r="LV33" s="0"/>
+      <c r="LW33" s="0"/>
+      <c r="LX33" s="0"/>
+      <c r="LY33" s="0"/>
+      <c r="LZ33" s="0"/>
+      <c r="MA33" s="0"/>
+      <c r="MB33" s="0"/>
+      <c r="MC33" s="0"/>
+      <c r="MD33" s="0"/>
+      <c r="ME33" s="0"/>
+      <c r="MF33" s="0"/>
+      <c r="MG33" s="0"/>
+      <c r="MH33" s="0"/>
+      <c r="MI33" s="0"/>
+      <c r="MJ33" s="0"/>
+      <c r="MK33" s="0"/>
+      <c r="ML33" s="0"/>
+      <c r="MM33" s="0"/>
+      <c r="MN33" s="0"/>
+      <c r="MO33" s="0"/>
+      <c r="MP33" s="0"/>
+      <c r="MQ33" s="0"/>
+      <c r="MR33" s="0"/>
+      <c r="MS33" s="0"/>
+      <c r="MT33" s="0"/>
+      <c r="MU33" s="0"/>
+      <c r="MV33" s="0"/>
+      <c r="MW33" s="0"/>
+      <c r="MX33" s="0"/>
+      <c r="MY33" s="0"/>
+      <c r="MZ33" s="0"/>
+      <c r="NA33" s="0"/>
+      <c r="NB33" s="0"/>
+      <c r="NC33" s="0"/>
+      <c r="ND33" s="0"/>
+      <c r="NE33" s="0"/>
+      <c r="NF33" s="0"/>
+      <c r="NG33" s="0"/>
+      <c r="NH33" s="0"/>
+      <c r="NI33" s="0"/>
+      <c r="NJ33" s="0"/>
+      <c r="NK33" s="0"/>
+      <c r="NL33" s="0"/>
+      <c r="NM33" s="0"/>
+      <c r="NN33" s="0"/>
+      <c r="NO33" s="0"/>
+      <c r="NP33" s="0"/>
+      <c r="NQ33" s="0"/>
+      <c r="NR33" s="0"/>
+      <c r="NS33" s="0"/>
+      <c r="NT33" s="0"/>
+      <c r="NU33" s="0"/>
+      <c r="NV33" s="0"/>
+      <c r="NW33" s="0"/>
+      <c r="NX33" s="0"/>
+      <c r="NY33" s="0"/>
+      <c r="NZ33" s="0"/>
+      <c r="OA33" s="0"/>
+      <c r="OB33" s="0"/>
+      <c r="OC33" s="0"/>
+      <c r="OD33" s="0"/>
+      <c r="OE33" s="0"/>
+      <c r="OF33" s="0"/>
+      <c r="OG33" s="0"/>
+      <c r="OH33" s="0"/>
+      <c r="OI33" s="0"/>
+      <c r="OJ33" s="0"/>
+      <c r="OK33" s="0"/>
+      <c r="OL33" s="0"/>
+      <c r="OM33" s="0"/>
+      <c r="ON33" s="0"/>
+      <c r="OO33" s="0"/>
+      <c r="OP33" s="0"/>
+      <c r="OQ33" s="0"/>
+      <c r="OR33" s="0"/>
+      <c r="OS33" s="0"/>
+      <c r="OT33" s="0"/>
+      <c r="OU33" s="0"/>
+      <c r="OV33" s="0"/>
+      <c r="OW33" s="0"/>
+      <c r="OX33" s="0"/>
+      <c r="OY33" s="0"/>
+      <c r="OZ33" s="0"/>
+      <c r="PA33" s="0"/>
+      <c r="PB33" s="0"/>
+      <c r="PC33" s="0"/>
+      <c r="PD33" s="0"/>
+      <c r="PE33" s="0"/>
+      <c r="PF33" s="0"/>
+      <c r="PG33" s="0"/>
+      <c r="PH33" s="0"/>
+      <c r="PI33" s="0"/>
+      <c r="PJ33" s="0"/>
+      <c r="PK33" s="0"/>
+      <c r="PL33" s="0"/>
+      <c r="PM33" s="0"/>
+      <c r="PN33" s="0"/>
+      <c r="PO33" s="0"/>
+      <c r="PP33" s="0"/>
+      <c r="PQ33" s="0"/>
+      <c r="PR33" s="0"/>
+      <c r="PS33" s="0"/>
+      <c r="PT33" s="0"/>
+      <c r="PU33" s="0"/>
+      <c r="PV33" s="0"/>
+      <c r="PW33" s="0"/>
+      <c r="PX33" s="0"/>
+      <c r="PY33" s="0"/>
+      <c r="PZ33" s="0"/>
+      <c r="QA33" s="0"/>
+      <c r="QB33" s="0"/>
+      <c r="QC33" s="0"/>
+      <c r="QD33" s="0"/>
+      <c r="QE33" s="0"/>
+      <c r="QF33" s="0"/>
+      <c r="QG33" s="0"/>
+      <c r="QH33" s="0"/>
+      <c r="QI33" s="0"/>
+      <c r="QJ33" s="0"/>
+      <c r="QK33" s="0"/>
+      <c r="QL33" s="0"/>
+      <c r="QM33" s="0"/>
+      <c r="QN33" s="0"/>
+      <c r="QO33" s="0"/>
+      <c r="QP33" s="0"/>
+      <c r="QQ33" s="0"/>
+      <c r="QR33" s="0"/>
+      <c r="QS33" s="0"/>
+      <c r="QT33" s="0"/>
+      <c r="QU33" s="0"/>
+      <c r="QV33" s="0"/>
+      <c r="QW33" s="0"/>
+      <c r="QX33" s="0"/>
+      <c r="QY33" s="0"/>
+      <c r="QZ33" s="0"/>
+      <c r="RA33" s="0"/>
+      <c r="RB33" s="0"/>
+      <c r="RC33" s="0"/>
+      <c r="RD33" s="0"/>
+      <c r="RE33" s="0"/>
+      <c r="RF33" s="0"/>
+      <c r="RG33" s="0"/>
+      <c r="RH33" s="0"/>
+      <c r="RI33" s="0"/>
+      <c r="RJ33" s="0"/>
+      <c r="RK33" s="0"/>
+      <c r="RL33" s="0"/>
+      <c r="RM33" s="0"/>
+      <c r="RN33" s="0"/>
+      <c r="RO33" s="0"/>
+      <c r="RP33" s="0"/>
+      <c r="RQ33" s="0"/>
+      <c r="RR33" s="0"/>
+      <c r="RS33" s="0"/>
+      <c r="RT33" s="0"/>
+      <c r="RU33" s="0"/>
+      <c r="RV33" s="0"/>
+      <c r="RW33" s="0"/>
+      <c r="RX33" s="0"/>
+      <c r="RY33" s="0"/>
+      <c r="RZ33" s="0"/>
+      <c r="SA33" s="0"/>
+      <c r="SB33" s="0"/>
+      <c r="SC33" s="0"/>
+      <c r="SD33" s="0"/>
+      <c r="SE33" s="0"/>
+      <c r="SF33" s="0"/>
+      <c r="SG33" s="0"/>
+      <c r="SH33" s="0"/>
+      <c r="SI33" s="0"/>
+      <c r="SJ33" s="0"/>
+      <c r="SK33" s="0"/>
+      <c r="SL33" s="0"/>
+      <c r="SM33" s="0"/>
+      <c r="SN33" s="0"/>
+      <c r="SO33" s="0"/>
+      <c r="SP33" s="0"/>
+      <c r="SQ33" s="0"/>
+      <c r="SR33" s="0"/>
+      <c r="SS33" s="0"/>
+      <c r="ST33" s="0"/>
+      <c r="SU33" s="0"/>
+      <c r="SV33" s="0"/>
+      <c r="SW33" s="0"/>
+      <c r="SX33" s="0"/>
+      <c r="SY33" s="0"/>
+      <c r="SZ33" s="0"/>
+      <c r="TA33" s="0"/>
+      <c r="TB33" s="0"/>
+      <c r="TC33" s="0"/>
+      <c r="TD33" s="0"/>
+      <c r="TE33" s="0"/>
+      <c r="TF33" s="0"/>
+      <c r="TG33" s="0"/>
+      <c r="TH33" s="0"/>
+      <c r="TI33" s="0"/>
+      <c r="TJ33" s="0"/>
+      <c r="TK33" s="0"/>
+      <c r="TL33" s="0"/>
+      <c r="TM33" s="0"/>
+      <c r="TN33" s="0"/>
+      <c r="TO33" s="0"/>
+      <c r="TP33" s="0"/>
+      <c r="TQ33" s="0"/>
+      <c r="TR33" s="0"/>
+      <c r="TS33" s="0"/>
+      <c r="TT33" s="0"/>
+      <c r="TU33" s="0"/>
+      <c r="TV33" s="0"/>
+      <c r="TW33" s="0"/>
+      <c r="TX33" s="0"/>
+      <c r="TY33" s="0"/>
+      <c r="TZ33" s="0"/>
+      <c r="UA33" s="0"/>
+      <c r="UB33" s="0"/>
+      <c r="UC33" s="0"/>
+      <c r="UD33" s="0"/>
+      <c r="UE33" s="0"/>
+      <c r="UF33" s="0"/>
+      <c r="UG33" s="0"/>
+      <c r="UH33" s="0"/>
+      <c r="UI33" s="0"/>
+      <c r="UJ33" s="0"/>
+      <c r="UK33" s="0"/>
+      <c r="UL33" s="0"/>
+      <c r="UM33" s="0"/>
+      <c r="UN33" s="0"/>
+      <c r="UO33" s="0"/>
+      <c r="UP33" s="0"/>
+      <c r="UQ33" s="0"/>
+      <c r="UR33" s="0"/>
+      <c r="US33" s="0"/>
+      <c r="UT33" s="0"/>
+      <c r="UU33" s="0"/>
+      <c r="UV33" s="0"/>
+      <c r="UW33" s="0"/>
+      <c r="UX33" s="0"/>
+      <c r="UY33" s="0"/>
+      <c r="UZ33" s="0"/>
+      <c r="VA33" s="0"/>
+      <c r="VB33" s="0"/>
+      <c r="VC33" s="0"/>
+      <c r="VD33" s="0"/>
+      <c r="VE33" s="0"/>
+      <c r="VF33" s="0"/>
+      <c r="VG33" s="0"/>
+      <c r="VH33" s="0"/>
+      <c r="VI33" s="0"/>
+      <c r="VJ33" s="0"/>
+      <c r="VK33" s="0"/>
+      <c r="VL33" s="0"/>
+      <c r="VM33" s="0"/>
+      <c r="VN33" s="0"/>
+      <c r="VO33" s="0"/>
+      <c r="VP33" s="0"/>
+      <c r="VQ33" s="0"/>
+      <c r="VR33" s="0"/>
+      <c r="VS33" s="0"/>
+      <c r="VT33" s="0"/>
+      <c r="VU33" s="0"/>
+      <c r="VV33" s="0"/>
+      <c r="VW33" s="0"/>
+      <c r="VX33" s="0"/>
+      <c r="VY33" s="0"/>
+      <c r="VZ33" s="0"/>
+      <c r="WA33" s="0"/>
+      <c r="WB33" s="0"/>
+      <c r="WC33" s="0"/>
+      <c r="WD33" s="0"/>
+      <c r="WE33" s="0"/>
+      <c r="WF33" s="0"/>
+      <c r="WG33" s="0"/>
+      <c r="WH33" s="0"/>
+      <c r="WI33" s="0"/>
+      <c r="WJ33" s="0"/>
+      <c r="WK33" s="0"/>
+      <c r="WL33" s="0"/>
+      <c r="WM33" s="0"/>
+      <c r="WN33" s="0"/>
+      <c r="WO33" s="0"/>
+      <c r="WP33" s="0"/>
+      <c r="WQ33" s="0"/>
+      <c r="WR33" s="0"/>
+      <c r="WS33" s="0"/>
+      <c r="WT33" s="0"/>
+      <c r="WU33" s="0"/>
+      <c r="WV33" s="0"/>
+      <c r="WW33" s="0"/>
+      <c r="WX33" s="0"/>
+      <c r="WY33" s="0"/>
+      <c r="WZ33" s="0"/>
+      <c r="XA33" s="0"/>
+      <c r="XB33" s="0"/>
+      <c r="XC33" s="0"/>
+      <c r="XD33" s="0"/>
+      <c r="XE33" s="0"/>
+      <c r="XF33" s="0"/>
+      <c r="XG33" s="0"/>
+      <c r="XH33" s="0"/>
+      <c r="XI33" s="0"/>
+      <c r="XJ33" s="0"/>
+      <c r="XK33" s="0"/>
+      <c r="XL33" s="0"/>
+      <c r="XM33" s="0"/>
+      <c r="XN33" s="0"/>
+      <c r="XO33" s="0"/>
+      <c r="XP33" s="0"/>
+      <c r="XQ33" s="0"/>
+      <c r="XR33" s="0"/>
+      <c r="XS33" s="0"/>
+      <c r="XT33" s="0"/>
+      <c r="XU33" s="0"/>
+      <c r="XV33" s="0"/>
+      <c r="XW33" s="0"/>
+      <c r="XX33" s="0"/>
+      <c r="XY33" s="0"/>
+      <c r="XZ33" s="0"/>
+      <c r="YA33" s="0"/>
+      <c r="YB33" s="0"/>
+      <c r="YC33" s="0"/>
+      <c r="YD33" s="0"/>
+      <c r="YE33" s="0"/>
+      <c r="YF33" s="0"/>
+      <c r="YG33" s="0"/>
+      <c r="YH33" s="0"/>
+      <c r="YI33" s="0"/>
+      <c r="YJ33" s="0"/>
+      <c r="YK33" s="0"/>
+      <c r="YL33" s="0"/>
+      <c r="YM33" s="0"/>
+      <c r="YN33" s="0"/>
+      <c r="YO33" s="0"/>
+      <c r="YP33" s="0"/>
+      <c r="YQ33" s="0"/>
+      <c r="YR33" s="0"/>
+      <c r="YS33" s="0"/>
+      <c r="YT33" s="0"/>
+      <c r="YU33" s="0"/>
+      <c r="YV33" s="0"/>
+      <c r="YW33" s="0"/>
+      <c r="YX33" s="0"/>
+      <c r="YY33" s="0"/>
+      <c r="YZ33" s="0"/>
+      <c r="ZA33" s="0"/>
+      <c r="ZB33" s="0"/>
+      <c r="ZC33" s="0"/>
+      <c r="ZD33" s="0"/>
+      <c r="ZE33" s="0"/>
+      <c r="ZF33" s="0"/>
+      <c r="ZG33" s="0"/>
+      <c r="ZH33" s="0"/>
+      <c r="ZI33" s="0"/>
+      <c r="ZJ33" s="0"/>
+      <c r="ZK33" s="0"/>
+      <c r="ZL33" s="0"/>
+      <c r="ZM33" s="0"/>
+      <c r="ZN33" s="0"/>
+      <c r="ZO33" s="0"/>
+      <c r="ZP33" s="0"/>
+      <c r="ZQ33" s="0"/>
+      <c r="ZR33" s="0"/>
+      <c r="ZS33" s="0"/>
+      <c r="ZT33" s="0"/>
+      <c r="ZU33" s="0"/>
+      <c r="ZV33" s="0"/>
+      <c r="ZW33" s="0"/>
+      <c r="ZX33" s="0"/>
+      <c r="ZY33" s="0"/>
+      <c r="ZZ33" s="0"/>
+      <c r="AAA33" s="0"/>
+      <c r="AAB33" s="0"/>
+      <c r="AAC33" s="0"/>
+      <c r="AAD33" s="0"/>
+      <c r="AAE33" s="0"/>
+      <c r="AAF33" s="0"/>
+      <c r="AAG33" s="0"/>
+      <c r="AAH33" s="0"/>
+      <c r="AAI33" s="0"/>
+      <c r="AAJ33" s="0"/>
+      <c r="AAK33" s="0"/>
+      <c r="AAL33" s="0"/>
+      <c r="AAM33" s="0"/>
+      <c r="AAN33" s="0"/>
+      <c r="AAO33" s="0"/>
+      <c r="AAP33" s="0"/>
+      <c r="AAQ33" s="0"/>
+      <c r="AAR33" s="0"/>
+      <c r="AAS33" s="0"/>
+      <c r="AAT33" s="0"/>
+      <c r="AAU33" s="0"/>
+      <c r="AAV33" s="0"/>
+      <c r="AAW33" s="0"/>
+      <c r="AAX33" s="0"/>
+      <c r="AAY33" s="0"/>
+      <c r="AAZ33" s="0"/>
+      <c r="ABA33" s="0"/>
+      <c r="ABB33" s="0"/>
+      <c r="ABC33" s="0"/>
+      <c r="ABD33" s="0"/>
+      <c r="ABE33" s="0"/>
+      <c r="ABF33" s="0"/>
+      <c r="ABG33" s="0"/>
+      <c r="ABH33" s="0"/>
+      <c r="ABI33" s="0"/>
+      <c r="ABJ33" s="0"/>
+      <c r="ABK33" s="0"/>
+      <c r="ABL33" s="0"/>
+      <c r="ABM33" s="0"/>
+      <c r="ABN33" s="0"/>
+      <c r="ABO33" s="0"/>
+      <c r="ABP33" s="0"/>
+      <c r="ABQ33" s="0"/>
+      <c r="ABR33" s="0"/>
+      <c r="ABS33" s="0"/>
+      <c r="ABT33" s="0"/>
+      <c r="ABU33" s="0"/>
+      <c r="ABV33" s="0"/>
+      <c r="ABW33" s="0"/>
+      <c r="ABX33" s="0"/>
+      <c r="ABY33" s="0"/>
+      <c r="ABZ33" s="0"/>
+      <c r="ACA33" s="0"/>
+      <c r="ACB33" s="0"/>
+      <c r="ACC33" s="0"/>
+      <c r="ACD33" s="0"/>
+      <c r="ACE33" s="0"/>
+      <c r="ACF33" s="0"/>
+      <c r="ACG33" s="0"/>
+      <c r="ACH33" s="0"/>
+      <c r="ACI33" s="0"/>
+      <c r="ACJ33" s="0"/>
+      <c r="ACK33" s="0"/>
+      <c r="ACL33" s="0"/>
+      <c r="ACM33" s="0"/>
+      <c r="ACN33" s="0"/>
+      <c r="ACO33" s="0"/>
+      <c r="ACP33" s="0"/>
+      <c r="ACQ33" s="0"/>
+      <c r="ACR33" s="0"/>
+      <c r="ACS33" s="0"/>
+      <c r="ACT33" s="0"/>
+      <c r="ACU33" s="0"/>
+      <c r="ACV33" s="0"/>
+      <c r="ACW33" s="0"/>
+      <c r="ACX33" s="0"/>
+      <c r="ACY33" s="0"/>
+      <c r="ACZ33" s="0"/>
+      <c r="ADA33" s="0"/>
+      <c r="ADB33" s="0"/>
+      <c r="ADC33" s="0"/>
+      <c r="ADD33" s="0"/>
+      <c r="ADE33" s="0"/>
+      <c r="ADF33" s="0"/>
+      <c r="ADG33" s="0"/>
+      <c r="ADH33" s="0"/>
+      <c r="ADI33" s="0"/>
+      <c r="ADJ33" s="0"/>
+      <c r="ADK33" s="0"/>
+      <c r="ADL33" s="0"/>
+      <c r="ADM33" s="0"/>
+      <c r="ADN33" s="0"/>
+      <c r="ADO33" s="0"/>
+      <c r="ADP33" s="0"/>
+      <c r="ADQ33" s="0"/>
+      <c r="ADR33" s="0"/>
+      <c r="ADS33" s="0"/>
+      <c r="ADT33" s="0"/>
+      <c r="ADU33" s="0"/>
+      <c r="ADV33" s="0"/>
+      <c r="ADW33" s="0"/>
+      <c r="ADX33" s="0"/>
+      <c r="ADY33" s="0"/>
+      <c r="ADZ33" s="0"/>
+      <c r="AEA33" s="0"/>
+      <c r="AEB33" s="0"/>
+      <c r="AEC33" s="0"/>
+      <c r="AED33" s="0"/>
+      <c r="AEE33" s="0"/>
+      <c r="AEF33" s="0"/>
+      <c r="AEG33" s="0"/>
+      <c r="AEH33" s="0"/>
+      <c r="AEI33" s="0"/>
+      <c r="AEJ33" s="0"/>
+      <c r="AEK33" s="0"/>
+      <c r="AEL33" s="0"/>
+      <c r="AEM33" s="0"/>
+      <c r="AEN33" s="0"/>
+      <c r="AEO33" s="0"/>
+      <c r="AEP33" s="0"/>
+      <c r="AEQ33" s="0"/>
+      <c r="AER33" s="0"/>
+      <c r="AES33" s="0"/>
+      <c r="AET33" s="0"/>
+      <c r="AEU33" s="0"/>
+      <c r="AEV33" s="0"/>
+      <c r="AEW33" s="0"/>
+      <c r="AEX33" s="0"/>
+      <c r="AEY33" s="0"/>
+      <c r="AEZ33" s="0"/>
+      <c r="AFA33" s="0"/>
+      <c r="AFB33" s="0"/>
+      <c r="AFC33" s="0"/>
+      <c r="AFD33" s="0"/>
+      <c r="AFE33" s="0"/>
+      <c r="AFF33" s="0"/>
+      <c r="AFG33" s="0"/>
+      <c r="AFH33" s="0"/>
+      <c r="AFI33" s="0"/>
+      <c r="AFJ33" s="0"/>
+      <c r="AFK33" s="0"/>
+      <c r="AFL33" s="0"/>
+      <c r="AFM33" s="0"/>
+      <c r="AFN33" s="0"/>
+      <c r="AFO33" s="0"/>
+      <c r="AFP33" s="0"/>
+      <c r="AFQ33" s="0"/>
+      <c r="AFR33" s="0"/>
+      <c r="AFS33" s="0"/>
+      <c r="AFT33" s="0"/>
+      <c r="AFU33" s="0"/>
+      <c r="AFV33" s="0"/>
+      <c r="AFW33" s="0"/>
+      <c r="AFX33" s="0"/>
+      <c r="AFY33" s="0"/>
+      <c r="AFZ33" s="0"/>
+      <c r="AGA33" s="0"/>
+      <c r="AGB33" s="0"/>
+      <c r="AGC33" s="0"/>
+      <c r="AGD33" s="0"/>
+      <c r="AGE33" s="0"/>
+      <c r="AGF33" s="0"/>
+      <c r="AGG33" s="0"/>
+      <c r="AGH33" s="0"/>
+      <c r="AGI33" s="0"/>
+      <c r="AGJ33" s="0"/>
+      <c r="AGK33" s="0"/>
+      <c r="AGL33" s="0"/>
+      <c r="AGM33" s="0"/>
+      <c r="AGN33" s="0"/>
+      <c r="AGO33" s="0"/>
+      <c r="AGP33" s="0"/>
+      <c r="AGQ33" s="0"/>
+      <c r="AGR33" s="0"/>
+      <c r="AGS33" s="0"/>
+      <c r="AGT33" s="0"/>
+      <c r="AGU33" s="0"/>
+      <c r="AGV33" s="0"/>
+      <c r="AGW33" s="0"/>
+      <c r="AGX33" s="0"/>
+      <c r="AGY33" s="0"/>
+      <c r="AGZ33" s="0"/>
+      <c r="AHA33" s="0"/>
+      <c r="AHB33" s="0"/>
+      <c r="AHC33" s="0"/>
+      <c r="AHD33" s="0"/>
+      <c r="AHE33" s="0"/>
+      <c r="AHF33" s="0"/>
+      <c r="AHG33" s="0"/>
+      <c r="AHH33" s="0"/>
+      <c r="AHI33" s="0"/>
+      <c r="AHJ33" s="0"/>
+      <c r="AHK33" s="0"/>
+      <c r="AHL33" s="0"/>
+      <c r="AHM33" s="0"/>
+      <c r="AHN33" s="0"/>
+      <c r="AHO33" s="0"/>
+      <c r="AHP33" s="0"/>
+      <c r="AHQ33" s="0"/>
+      <c r="AHR33" s="0"/>
+      <c r="AHS33" s="0"/>
+      <c r="AHT33" s="0"/>
+      <c r="AHU33" s="0"/>
+      <c r="AHV33" s="0"/>
+      <c r="AHW33" s="0"/>
+      <c r="AHX33" s="0"/>
+      <c r="AHY33" s="0"/>
+      <c r="AHZ33" s="0"/>
+      <c r="AIA33" s="0"/>
+      <c r="AIB33" s="0"/>
+      <c r="AIC33" s="0"/>
+      <c r="AID33" s="0"/>
+      <c r="AIE33" s="0"/>
+      <c r="AIF33" s="0"/>
+      <c r="AIG33" s="0"/>
+      <c r="AIH33" s="0"/>
+      <c r="AII33" s="0"/>
+      <c r="AIJ33" s="0"/>
+      <c r="AIK33" s="0"/>
+      <c r="AIL33" s="0"/>
+      <c r="AIM33" s="0"/>
+      <c r="AIN33" s="0"/>
+      <c r="AIO33" s="0"/>
+      <c r="AIP33" s="0"/>
+      <c r="AIQ33" s="0"/>
+      <c r="AIR33" s="0"/>
+      <c r="AIS33" s="0"/>
+      <c r="AIT33" s="0"/>
+      <c r="AIU33" s="0"/>
+      <c r="AIV33" s="0"/>
+      <c r="AIW33" s="0"/>
+      <c r="AIX33" s="0"/>
+      <c r="AIY33" s="0"/>
+      <c r="AIZ33" s="0"/>
+      <c r="AJA33" s="0"/>
+      <c r="AJB33" s="0"/>
+      <c r="AJC33" s="0"/>
+      <c r="AJD33" s="0"/>
+      <c r="AJE33" s="0"/>
+      <c r="AJF33" s="0"/>
+      <c r="AJG33" s="0"/>
+      <c r="AJH33" s="0"/>
+      <c r="AJI33" s="0"/>
+      <c r="AJJ33" s="0"/>
+      <c r="AJK33" s="0"/>
+      <c r="AJL33" s="0"/>
+      <c r="AJM33" s="0"/>
+      <c r="AJN33" s="0"/>
+      <c r="AJO33" s="0"/>
+      <c r="AJP33" s="0"/>
+      <c r="AJQ33" s="0"/>
+      <c r="AJR33" s="0"/>
+      <c r="AJS33" s="0"/>
+      <c r="AJT33" s="0"/>
+      <c r="AJU33" s="0"/>
+      <c r="AJV33" s="0"/>
+      <c r="AJW33" s="0"/>
+      <c r="AJX33" s="0"/>
+      <c r="AJY33" s="0"/>
+      <c r="AJZ33" s="0"/>
+      <c r="AKA33" s="0"/>
+      <c r="AKB33" s="0"/>
+      <c r="AKC33" s="0"/>
+      <c r="AKD33" s="0"/>
+      <c r="AKE33" s="0"/>
+      <c r="AKF33" s="0"/>
+      <c r="AKG33" s="0"/>
+      <c r="AKH33" s="0"/>
+      <c r="AKI33" s="0"/>
+      <c r="AKJ33" s="0"/>
+      <c r="AKK33" s="0"/>
+      <c r="AKL33" s="0"/>
+      <c r="AKM33" s="0"/>
+      <c r="AKN33" s="0"/>
+      <c r="AKO33" s="0"/>
+      <c r="AKP33" s="0"/>
+      <c r="AKQ33" s="0"/>
+      <c r="AKR33" s="0"/>
+      <c r="AKS33" s="0"/>
+      <c r="AKT33" s="0"/>
+      <c r="AKU33" s="0"/>
+      <c r="AKV33" s="0"/>
+      <c r="AKW33" s="0"/>
+      <c r="AKX33" s="0"/>
+      <c r="AKY33" s="0"/>
+      <c r="AKZ33" s="0"/>
+      <c r="ALA33" s="0"/>
+      <c r="ALB33" s="0"/>
+      <c r="ALC33" s="0"/>
+      <c r="ALD33" s="0"/>
+      <c r="ALE33" s="0"/>
+      <c r="ALF33" s="0"/>
+      <c r="ALG33" s="0"/>
+      <c r="ALH33" s="0"/>
+      <c r="ALI33" s="0"/>
+      <c r="ALJ33" s="0"/>
+      <c r="ALK33" s="0"/>
+      <c r="ALL33" s="0"/>
+      <c r="ALM33" s="0"/>
+      <c r="ALN33" s="0"/>
+      <c r="ALO33" s="0"/>
+      <c r="ALP33" s="0"/>
+      <c r="ALQ33" s="0"/>
+      <c r="ALR33" s="0"/>
+      <c r="ALS33" s="0"/>
+      <c r="ALT33" s="0"/>
+      <c r="ALU33" s="0"/>
+      <c r="ALV33" s="0"/>
+      <c r="ALW33" s="0"/>
+      <c r="ALX33" s="0"/>
+      <c r="ALY33" s="0"/>
+      <c r="ALZ33" s="0"/>
+      <c r="AMA33" s="0"/>
+      <c r="AMB33" s="0"/>
+      <c r="AMC33" s="0"/>
+      <c r="AMD33" s="0"/>
+      <c r="AME33" s="0"/>
+      <c r="AMF33" s="0"/>
+      <c r="AMG33" s="0"/>
+      <c r="AMH33" s="0"/>
+      <c r="AMI33" s="0"/>
+      <c r="AMJ33" s="0"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0"/>
+      <c r="B34" s="0"/>
+      <c r="C34" s="0"/>
+      <c r="D34" s="0"/>
+      <c r="E34" s="0"/>
+      <c r="F34" s="0"/>
+      <c r="G34" s="0"/>
+      <c r="H34" s="0"/>
+      <c r="I34" s="0"/>
+      <c r="J34" s="0"/>
+      <c r="K34" s="0"/>
+      <c r="L34" s="0"/>
+      <c r="M34" s="0"/>
+      <c r="N34" s="0"/>
+      <c r="O34" s="0"/>
+      <c r="P34" s="0"/>
+      <c r="Q34" s="0"/>
+      <c r="R34" s="0"/>
+      <c r="S34" s="0"/>
+      <c r="T34" s="0"/>
+      <c r="U34" s="0"/>
+      <c r="V34" s="0"/>
+      <c r="W34" s="0"/>
+      <c r="X34" s="0"/>
+      <c r="Y34" s="0"/>
+      <c r="Z34" s="0"/>
+      <c r="AA34" s="0"/>
+      <c r="AB34" s="0"/>
+      <c r="AC34" s="0"/>
+      <c r="AD34" s="0"/>
+      <c r="AE34" s="0"/>
+      <c r="AF34" s="0"/>
+      <c r="AG34" s="0"/>
+      <c r="AH34" s="0"/>
+      <c r="AI34" s="0"/>
+      <c r="AJ34" s="0"/>
+      <c r="AK34" s="0"/>
+      <c r="AL34" s="0"/>
+      <c r="AM34" s="0"/>
+      <c r="AN34" s="0"/>
+      <c r="AO34" s="0"/>
+      <c r="AP34" s="0"/>
+      <c r="AQ34" s="0"/>
+      <c r="AR34" s="0"/>
+      <c r="AS34" s="0"/>
+      <c r="AT34" s="0"/>
+      <c r="AU34" s="0"/>
+      <c r="AV34" s="0"/>
+      <c r="AW34" s="0"/>
+      <c r="AX34" s="0"/>
+      <c r="AY34" s="0"/>
+      <c r="AZ34" s="0"/>
+      <c r="BA34" s="0"/>
+      <c r="BB34" s="0"/>
+      <c r="BC34" s="0"/>
+      <c r="BD34" s="0"/>
+      <c r="BE34" s="0"/>
+      <c r="BF34" s="0"/>
+      <c r="BG34" s="0"/>
+      <c r="BH34" s="0"/>
+      <c r="BI34" s="0"/>
+      <c r="BJ34" s="0"/>
+      <c r="BK34" s="0"/>
+      <c r="BL34" s="0"/>
+      <c r="BM34" s="0"/>
+      <c r="BN34" s="0"/>
+      <c r="BO34" s="0"/>
+      <c r="BP34" s="0"/>
+      <c r="BQ34" s="0"/>
+      <c r="BR34" s="0"/>
+      <c r="BS34" s="0"/>
+      <c r="BT34" s="0"/>
+      <c r="BU34" s="0"/>
+      <c r="BV34" s="0"/>
+      <c r="BW34" s="0"/>
+      <c r="BX34" s="0"/>
+      <c r="BY34" s="0"/>
+      <c r="BZ34" s="0"/>
+      <c r="CA34" s="0"/>
+      <c r="CB34" s="0"/>
+      <c r="CC34" s="0"/>
+      <c r="CD34" s="0"/>
+      <c r="CE34" s="0"/>
+      <c r="CF34" s="0"/>
+      <c r="CG34" s="0"/>
+      <c r="CH34" s="0"/>
+      <c r="CI34" s="0"/>
+      <c r="CJ34" s="0"/>
+      <c r="CK34" s="0"/>
+      <c r="CL34" s="0"/>
+      <c r="CM34" s="0"/>
+      <c r="CN34" s="0"/>
+      <c r="CO34" s="0"/>
+      <c r="CP34" s="0"/>
+      <c r="CQ34" s="0"/>
+      <c r="CR34" s="0"/>
+      <c r="CS34" s="0"/>
+      <c r="CT34" s="0"/>
+      <c r="CU34" s="0"/>
+      <c r="CV34" s="0"/>
+      <c r="CW34" s="0"/>
+      <c r="CX34" s="0"/>
+      <c r="CY34" s="0"/>
+      <c r="CZ34" s="0"/>
+      <c r="DA34" s="0"/>
+      <c r="DB34" s="0"/>
+      <c r="DC34" s="0"/>
+      <c r="DD34" s="0"/>
+      <c r="DE34" s="0"/>
+      <c r="DF34" s="0"/>
+      <c r="DG34" s="0"/>
+      <c r="DH34" s="0"/>
+      <c r="DI34" s="0"/>
+      <c r="DJ34" s="0"/>
+      <c r="DK34" s="0"/>
+      <c r="DL34" s="0"/>
+      <c r="DM34" s="0"/>
+      <c r="DN34" s="0"/>
+      <c r="DO34" s="0"/>
+      <c r="DP34" s="0"/>
+      <c r="DQ34" s="0"/>
+      <c r="DR34" s="0"/>
+      <c r="DS34" s="0"/>
+      <c r="DT34" s="0"/>
+      <c r="DU34" s="0"/>
+      <c r="DV34" s="0"/>
+      <c r="DW34" s="0"/>
+      <c r="DX34" s="0"/>
+      <c r="DY34" s="0"/>
+      <c r="DZ34" s="0"/>
+      <c r="EA34" s="0"/>
+      <c r="EB34" s="0"/>
+      <c r="EC34" s="0"/>
+      <c r="ED34" s="0"/>
+      <c r="EE34" s="0"/>
+      <c r="EF34" s="0"/>
+      <c r="EG34" s="0"/>
+      <c r="EH34" s="0"/>
+      <c r="EI34" s="0"/>
+      <c r="EJ34" s="0"/>
+      <c r="EK34" s="0"/>
+      <c r="EL34" s="0"/>
+      <c r="EM34" s="0"/>
+      <c r="EN34" s="0"/>
+      <c r="EO34" s="0"/>
+      <c r="EP34" s="0"/>
+      <c r="EQ34" s="0"/>
+      <c r="ER34" s="0"/>
+      <c r="ES34" s="0"/>
+      <c r="ET34" s="0"/>
+      <c r="EU34" s="0"/>
+      <c r="EV34" s="0"/>
+      <c r="EW34" s="0"/>
+      <c r="EX34" s="0"/>
+      <c r="EY34" s="0"/>
+      <c r="EZ34" s="0"/>
+      <c r="FA34" s="0"/>
+      <c r="FB34" s="0"/>
+      <c r="FC34" s="0"/>
+      <c r="FD34" s="0"/>
+      <c r="FE34" s="0"/>
+      <c r="FF34" s="0"/>
+      <c r="FG34" s="0"/>
+      <c r="FH34" s="0"/>
+      <c r="FI34" s="0"/>
+      <c r="FJ34" s="0"/>
+      <c r="FK34" s="0"/>
+      <c r="FL34" s="0"/>
+      <c r="FM34" s="0"/>
+      <c r="FN34" s="0"/>
+      <c r="FO34" s="0"/>
+      <c r="FP34" s="0"/>
+      <c r="FQ34" s="0"/>
+      <c r="FR34" s="0"/>
+      <c r="FS34" s="0"/>
+      <c r="FT34" s="0"/>
+      <c r="FU34" s="0"/>
+      <c r="FV34" s="0"/>
+      <c r="FW34" s="0"/>
+      <c r="FX34" s="0"/>
+      <c r="FY34" s="0"/>
+      <c r="FZ34" s="0"/>
+      <c r="GA34" s="0"/>
+      <c r="GB34" s="0"/>
+      <c r="GC34" s="0"/>
+      <c r="GD34" s="0"/>
+      <c r="GE34" s="0"/>
+      <c r="GF34" s="0"/>
+      <c r="GG34" s="0"/>
+      <c r="GH34" s="0"/>
+      <c r="GI34" s="0"/>
+      <c r="GJ34" s="0"/>
+      <c r="GK34" s="0"/>
+      <c r="GL34" s="0"/>
+      <c r="GM34" s="0"/>
+      <c r="GN34" s="0"/>
+      <c r="GO34" s="0"/>
+      <c r="GP34" s="0"/>
+      <c r="GQ34" s="0"/>
+      <c r="GR34" s="0"/>
+      <c r="GS34" s="0"/>
+      <c r="GT34" s="0"/>
+      <c r="GU34" s="0"/>
+      <c r="GV34" s="0"/>
+      <c r="GW34" s="0"/>
+      <c r="GX34" s="0"/>
+      <c r="GY34" s="0"/>
+      <c r="GZ34" s="0"/>
+      <c r="HA34" s="0"/>
+      <c r="HB34" s="0"/>
+      <c r="HC34" s="0"/>
+      <c r="HD34" s="0"/>
+      <c r="HE34" s="0"/>
+      <c r="HF34" s="0"/>
+      <c r="HG34" s="0"/>
+      <c r="HH34" s="0"/>
+      <c r="HI34" s="0"/>
+      <c r="HJ34" s="0"/>
+      <c r="HK34" s="0"/>
+      <c r="HL34" s="0"/>
+      <c r="HM34" s="0"/>
+      <c r="HN34" s="0"/>
+      <c r="HO34" s="0"/>
+      <c r="HP34" s="0"/>
+      <c r="HQ34" s="0"/>
+      <c r="HR34" s="0"/>
+      <c r="HS34" s="0"/>
+      <c r="HT34" s="0"/>
+      <c r="HU34" s="0"/>
+      <c r="HV34" s="0"/>
+      <c r="HW34" s="0"/>
+      <c r="HX34" s="0"/>
+      <c r="HY34" s="0"/>
+      <c r="HZ34" s="0"/>
+      <c r="IA34" s="0"/>
+      <c r="IB34" s="0"/>
+      <c r="IC34" s="0"/>
+      <c r="ID34" s="0"/>
+      <c r="IE34" s="0"/>
+      <c r="IF34" s="0"/>
+      <c r="IG34" s="0"/>
+      <c r="IH34" s="0"/>
+      <c r="II34" s="0"/>
+      <c r="IJ34" s="0"/>
+      <c r="IK34" s="0"/>
+      <c r="IL34" s="0"/>
+      <c r="IM34" s="0"/>
+      <c r="IN34" s="0"/>
+      <c r="IO34" s="0"/>
+      <c r="IP34" s="0"/>
+      <c r="IQ34" s="0"/>
+      <c r="IR34" s="0"/>
+      <c r="IS34" s="0"/>
+      <c r="IT34" s="0"/>
+      <c r="IU34" s="0"/>
+      <c r="IV34" s="0"/>
+      <c r="IW34" s="0"/>
+      <c r="IX34" s="0"/>
+      <c r="IY34" s="0"/>
+      <c r="IZ34" s="0"/>
+      <c r="JA34" s="0"/>
+      <c r="JB34" s="0"/>
+      <c r="JC34" s="0"/>
+      <c r="JD34" s="0"/>
+      <c r="JE34" s="0"/>
+      <c r="JF34" s="0"/>
+      <c r="JG34" s="0"/>
+      <c r="JH34" s="0"/>
+      <c r="JI34" s="0"/>
+      <c r="JJ34" s="0"/>
+      <c r="JK34" s="0"/>
+      <c r="JL34" s="0"/>
+      <c r="JM34" s="0"/>
+      <c r="JN34" s="0"/>
+      <c r="JO34" s="0"/>
+      <c r="JP34" s="0"/>
+      <c r="JQ34" s="0"/>
+      <c r="JR34" s="0"/>
+      <c r="JS34" s="0"/>
+      <c r="JT34" s="0"/>
+      <c r="JU34" s="0"/>
+      <c r="JV34" s="0"/>
+      <c r="JW34" s="0"/>
+      <c r="JX34" s="0"/>
+      <c r="JY34" s="0"/>
+      <c r="JZ34" s="0"/>
+      <c r="KA34" s="0"/>
+      <c r="KB34" s="0"/>
+      <c r="KC34" s="0"/>
+      <c r="KD34" s="0"/>
+      <c r="KE34" s="0"/>
+      <c r="KF34" s="0"/>
+      <c r="KG34" s="0"/>
+      <c r="KH34" s="0"/>
+      <c r="KI34" s="0"/>
+      <c r="KJ34" s="0"/>
+      <c r="KK34" s="0"/>
+      <c r="KL34" s="0"/>
+      <c r="KM34" s="0"/>
+      <c r="KN34" s="0"/>
+      <c r="KO34" s="0"/>
+      <c r="KP34" s="0"/>
+      <c r="KQ34" s="0"/>
+      <c r="KR34" s="0"/>
+      <c r="KS34" s="0"/>
+      <c r="KT34" s="0"/>
+      <c r="KU34" s="0"/>
+      <c r="KV34" s="0"/>
+      <c r="KW34" s="0"/>
+      <c r="KX34" s="0"/>
+      <c r="KY34" s="0"/>
+      <c r="KZ34" s="0"/>
+      <c r="LA34" s="0"/>
+      <c r="LB34" s="0"/>
+      <c r="LC34" s="0"/>
+      <c r="LD34" s="0"/>
+      <c r="LE34" s="0"/>
+      <c r="LF34" s="0"/>
+      <c r="LG34" s="0"/>
+      <c r="LH34" s="0"/>
+      <c r="LI34" s="0"/>
+      <c r="LJ34" s="0"/>
+      <c r="LK34" s="0"/>
+      <c r="LL34" s="0"/>
+      <c r="LM34" s="0"/>
+      <c r="LN34" s="0"/>
+      <c r="LO34" s="0"/>
+      <c r="LP34" s="0"/>
+      <c r="LQ34" s="0"/>
+      <c r="LR34" s="0"/>
+      <c r="LS34" s="0"/>
+      <c r="LT34" s="0"/>
+      <c r="LU34" s="0"/>
+      <c r="LV34" s="0"/>
+      <c r="LW34" s="0"/>
+      <c r="LX34" s="0"/>
+      <c r="LY34" s="0"/>
+      <c r="LZ34" s="0"/>
+      <c r="MA34" s="0"/>
+      <c r="MB34" s="0"/>
+      <c r="MC34" s="0"/>
+      <c r="MD34" s="0"/>
+      <c r="ME34" s="0"/>
+      <c r="MF34" s="0"/>
+      <c r="MG34" s="0"/>
+      <c r="MH34" s="0"/>
+      <c r="MI34" s="0"/>
+      <c r="MJ34" s="0"/>
+      <c r="MK34" s="0"/>
+      <c r="ML34" s="0"/>
+      <c r="MM34" s="0"/>
+      <c r="MN34" s="0"/>
+      <c r="MO34" s="0"/>
+      <c r="MP34" s="0"/>
+      <c r="MQ34" s="0"/>
+      <c r="MR34" s="0"/>
+      <c r="MS34" s="0"/>
+      <c r="MT34" s="0"/>
+      <c r="MU34" s="0"/>
+      <c r="MV34" s="0"/>
+      <c r="MW34" s="0"/>
+      <c r="MX34" s="0"/>
+      <c r="MY34" s="0"/>
+      <c r="MZ34" s="0"/>
+      <c r="NA34" s="0"/>
+      <c r="NB34" s="0"/>
+      <c r="NC34" s="0"/>
+      <c r="ND34" s="0"/>
+      <c r="NE34" s="0"/>
+      <c r="NF34" s="0"/>
+      <c r="NG34" s="0"/>
+      <c r="NH34" s="0"/>
+      <c r="NI34" s="0"/>
+      <c r="NJ34" s="0"/>
+      <c r="NK34" s="0"/>
+      <c r="NL34" s="0"/>
+      <c r="NM34" s="0"/>
+      <c r="NN34" s="0"/>
+      <c r="NO34" s="0"/>
+      <c r="NP34" s="0"/>
+      <c r="NQ34" s="0"/>
+      <c r="NR34" s="0"/>
+      <c r="NS34" s="0"/>
+      <c r="NT34" s="0"/>
+      <c r="NU34" s="0"/>
+      <c r="NV34" s="0"/>
+      <c r="NW34" s="0"/>
+      <c r="NX34" s="0"/>
+      <c r="NY34" s="0"/>
+      <c r="NZ34" s="0"/>
+      <c r="OA34" s="0"/>
+      <c r="OB34" s="0"/>
+      <c r="OC34" s="0"/>
+      <c r="OD34" s="0"/>
+      <c r="OE34" s="0"/>
+      <c r="OF34" s="0"/>
+      <c r="OG34" s="0"/>
+      <c r="OH34" s="0"/>
+      <c r="OI34" s="0"/>
+      <c r="OJ34" s="0"/>
+      <c r="OK34" s="0"/>
+      <c r="OL34" s="0"/>
+      <c r="OM34" s="0"/>
+      <c r="ON34" s="0"/>
+      <c r="OO34" s="0"/>
+      <c r="OP34" s="0"/>
+      <c r="OQ34" s="0"/>
+      <c r="OR34" s="0"/>
+      <c r="OS34" s="0"/>
+      <c r="OT34" s="0"/>
+      <c r="OU34" s="0"/>
+      <c r="OV34" s="0"/>
+      <c r="OW34" s="0"/>
+      <c r="OX34" s="0"/>
+      <c r="OY34" s="0"/>
+      <c r="OZ34" s="0"/>
+      <c r="PA34" s="0"/>
+      <c r="PB34" s="0"/>
+      <c r="PC34" s="0"/>
+      <c r="PD34" s="0"/>
+      <c r="PE34" s="0"/>
+      <c r="PF34" s="0"/>
+      <c r="PG34" s="0"/>
+      <c r="PH34" s="0"/>
+      <c r="PI34" s="0"/>
+      <c r="PJ34" s="0"/>
+      <c r="PK34" s="0"/>
+      <c r="PL34" s="0"/>
+      <c r="PM34" s="0"/>
+      <c r="PN34" s="0"/>
+      <c r="PO34" s="0"/>
+      <c r="PP34" s="0"/>
+      <c r="PQ34" s="0"/>
+      <c r="PR34" s="0"/>
+      <c r="PS34" s="0"/>
+      <c r="PT34" s="0"/>
+      <c r="PU34" s="0"/>
+      <c r="PV34" s="0"/>
+      <c r="PW34" s="0"/>
+      <c r="PX34" s="0"/>
+      <c r="PY34" s="0"/>
+      <c r="PZ34" s="0"/>
+      <c r="QA34" s="0"/>
+      <c r="QB34" s="0"/>
+      <c r="QC34" s="0"/>
+      <c r="QD34" s="0"/>
+      <c r="QE34" s="0"/>
+      <c r="QF34" s="0"/>
+      <c r="QG34" s="0"/>
+      <c r="QH34" s="0"/>
+      <c r="QI34" s="0"/>
+      <c r="QJ34" s="0"/>
+      <c r="QK34" s="0"/>
+      <c r="QL34" s="0"/>
+      <c r="QM34" s="0"/>
+      <c r="QN34" s="0"/>
+      <c r="QO34" s="0"/>
+      <c r="QP34" s="0"/>
+      <c r="QQ34" s="0"/>
+      <c r="QR34" s="0"/>
+      <c r="QS34" s="0"/>
+      <c r="QT34" s="0"/>
+      <c r="QU34" s="0"/>
+      <c r="QV34" s="0"/>
+      <c r="QW34" s="0"/>
+      <c r="QX34" s="0"/>
+      <c r="QY34" s="0"/>
+      <c r="QZ34" s="0"/>
+      <c r="RA34" s="0"/>
+      <c r="RB34" s="0"/>
+      <c r="RC34" s="0"/>
+      <c r="RD34" s="0"/>
+      <c r="RE34" s="0"/>
+      <c r="RF34" s="0"/>
+      <c r="RG34" s="0"/>
+      <c r="RH34" s="0"/>
+      <c r="RI34" s="0"/>
+      <c r="RJ34" s="0"/>
+      <c r="RK34" s="0"/>
+      <c r="RL34" s="0"/>
+      <c r="RM34" s="0"/>
+      <c r="RN34" s="0"/>
+      <c r="RO34" s="0"/>
+      <c r="RP34" s="0"/>
+      <c r="RQ34" s="0"/>
+      <c r="RR34" s="0"/>
+      <c r="RS34" s="0"/>
+      <c r="RT34" s="0"/>
+      <c r="RU34" s="0"/>
+      <c r="RV34" s="0"/>
+      <c r="RW34" s="0"/>
+      <c r="RX34" s="0"/>
+      <c r="RY34" s="0"/>
+      <c r="RZ34" s="0"/>
+      <c r="SA34" s="0"/>
+      <c r="SB34" s="0"/>
+      <c r="SC34" s="0"/>
+      <c r="SD34" s="0"/>
+      <c r="SE34" s="0"/>
+      <c r="SF34" s="0"/>
+      <c r="SG34" s="0"/>
+      <c r="SH34" s="0"/>
+      <c r="SI34" s="0"/>
+      <c r="SJ34" s="0"/>
+      <c r="SK34" s="0"/>
+      <c r="SL34" s="0"/>
+      <c r="SM34" s="0"/>
+      <c r="SN34" s="0"/>
+      <c r="SO34" s="0"/>
+      <c r="SP34" s="0"/>
+      <c r="SQ34" s="0"/>
+      <c r="SR34" s="0"/>
+      <c r="SS34" s="0"/>
+      <c r="ST34" s="0"/>
+      <c r="SU34" s="0"/>
+      <c r="SV34" s="0"/>
+      <c r="SW34" s="0"/>
+      <c r="SX34" s="0"/>
+      <c r="SY34" s="0"/>
+      <c r="SZ34" s="0"/>
+      <c r="TA34" s="0"/>
+      <c r="TB34" s="0"/>
+      <c r="TC34" s="0"/>
+      <c r="TD34" s="0"/>
+      <c r="TE34" s="0"/>
+      <c r="TF34" s="0"/>
+      <c r="TG34" s="0"/>
+      <c r="TH34" s="0"/>
+      <c r="TI34" s="0"/>
+      <c r="TJ34" s="0"/>
+      <c r="TK34" s="0"/>
+      <c r="TL34" s="0"/>
+      <c r="TM34" s="0"/>
+      <c r="TN34" s="0"/>
+      <c r="TO34" s="0"/>
+      <c r="TP34" s="0"/>
+      <c r="TQ34" s="0"/>
+      <c r="TR34" s="0"/>
+      <c r="TS34" s="0"/>
+      <c r="TT34" s="0"/>
+      <c r="TU34" s="0"/>
+      <c r="TV34" s="0"/>
+      <c r="TW34" s="0"/>
+      <c r="TX34" s="0"/>
+      <c r="TY34" s="0"/>
+      <c r="TZ34" s="0"/>
+      <c r="UA34" s="0"/>
+      <c r="UB34" s="0"/>
+      <c r="UC34" s="0"/>
+      <c r="UD34" s="0"/>
+      <c r="UE34" s="0"/>
+      <c r="UF34" s="0"/>
+      <c r="UG34" s="0"/>
+      <c r="UH34" s="0"/>
+      <c r="UI34" s="0"/>
+      <c r="UJ34" s="0"/>
+      <c r="UK34" s="0"/>
+      <c r="UL34" s="0"/>
+      <c r="UM34" s="0"/>
+      <c r="UN34" s="0"/>
+      <c r="UO34" s="0"/>
+      <c r="UP34" s="0"/>
+      <c r="UQ34" s="0"/>
+      <c r="UR34" s="0"/>
+      <c r="US34" s="0"/>
+      <c r="UT34" s="0"/>
+      <c r="UU34" s="0"/>
+      <c r="UV34" s="0"/>
+      <c r="UW34" s="0"/>
+      <c r="UX34" s="0"/>
+      <c r="UY34" s="0"/>
+      <c r="UZ34" s="0"/>
+      <c r="VA34" s="0"/>
+      <c r="VB34" s="0"/>
+      <c r="VC34" s="0"/>
+      <c r="VD34" s="0"/>
+      <c r="VE34" s="0"/>
+      <c r="VF34" s="0"/>
+      <c r="VG34" s="0"/>
+      <c r="VH34" s="0"/>
+      <c r="VI34" s="0"/>
+      <c r="VJ34" s="0"/>
+      <c r="VK34" s="0"/>
+      <c r="VL34" s="0"/>
+      <c r="VM34" s="0"/>
+      <c r="VN34" s="0"/>
+      <c r="VO34" s="0"/>
+      <c r="VP34" s="0"/>
+      <c r="VQ34" s="0"/>
+      <c r="VR34" s="0"/>
+      <c r="VS34" s="0"/>
+      <c r="VT34" s="0"/>
+      <c r="VU34" s="0"/>
+      <c r="VV34" s="0"/>
+      <c r="VW34" s="0"/>
+      <c r="VX34" s="0"/>
+      <c r="VY34" s="0"/>
+      <c r="VZ34" s="0"/>
+      <c r="WA34" s="0"/>
+      <c r="WB34" s="0"/>
+      <c r="WC34" s="0"/>
+      <c r="WD34" s="0"/>
+      <c r="WE34" s="0"/>
+      <c r="WF34" s="0"/>
+      <c r="WG34" s="0"/>
+      <c r="WH34" s="0"/>
+      <c r="WI34" s="0"/>
+      <c r="WJ34" s="0"/>
+      <c r="WK34" s="0"/>
+      <c r="WL34" s="0"/>
+      <c r="WM34" s="0"/>
+      <c r="WN34" s="0"/>
+      <c r="WO34" s="0"/>
+      <c r="WP34" s="0"/>
+      <c r="WQ34" s="0"/>
+      <c r="WR34" s="0"/>
+      <c r="WS34" s="0"/>
+      <c r="WT34" s="0"/>
+      <c r="WU34" s="0"/>
+      <c r="WV34" s="0"/>
+      <c r="WW34" s="0"/>
+      <c r="WX34" s="0"/>
+      <c r="WY34" s="0"/>
+      <c r="WZ34" s="0"/>
+      <c r="XA34" s="0"/>
+      <c r="XB34" s="0"/>
+      <c r="XC34" s="0"/>
+      <c r="XD34" s="0"/>
+      <c r="XE34" s="0"/>
+      <c r="XF34" s="0"/>
+      <c r="XG34" s="0"/>
+      <c r="XH34" s="0"/>
+      <c r="XI34" s="0"/>
+      <c r="XJ34" s="0"/>
+      <c r="XK34" s="0"/>
+      <c r="XL34" s="0"/>
+      <c r="XM34" s="0"/>
+      <c r="XN34" s="0"/>
+      <c r="XO34" s="0"/>
+      <c r="XP34" s="0"/>
+      <c r="XQ34" s="0"/>
+      <c r="XR34" s="0"/>
+      <c r="XS34" s="0"/>
+      <c r="XT34" s="0"/>
+      <c r="XU34" s="0"/>
+      <c r="XV34" s="0"/>
+      <c r="XW34" s="0"/>
+      <c r="XX34" s="0"/>
+      <c r="XY34" s="0"/>
+      <c r="XZ34" s="0"/>
+      <c r="YA34" s="0"/>
+      <c r="YB34" s="0"/>
+      <c r="YC34" s="0"/>
+      <c r="YD34" s="0"/>
+      <c r="YE34" s="0"/>
+      <c r="YF34" s="0"/>
+      <c r="YG34" s="0"/>
+      <c r="YH34" s="0"/>
+      <c r="YI34" s="0"/>
+      <c r="YJ34" s="0"/>
+      <c r="YK34" s="0"/>
+      <c r="YL34" s="0"/>
+      <c r="YM34" s="0"/>
+      <c r="YN34" s="0"/>
+      <c r="YO34" s="0"/>
+      <c r="YP34" s="0"/>
+      <c r="YQ34" s="0"/>
+      <c r="YR34" s="0"/>
+      <c r="YS34" s="0"/>
+      <c r="YT34" s="0"/>
+      <c r="YU34" s="0"/>
+      <c r="YV34" s="0"/>
+      <c r="YW34" s="0"/>
+      <c r="YX34" s="0"/>
+      <c r="YY34" s="0"/>
+      <c r="YZ34" s="0"/>
+      <c r="ZA34" s="0"/>
+      <c r="ZB34" s="0"/>
+      <c r="ZC34" s="0"/>
+      <c r="ZD34" s="0"/>
+      <c r="ZE34" s="0"/>
+      <c r="ZF34" s="0"/>
+      <c r="ZG34" s="0"/>
+      <c r="ZH34" s="0"/>
+      <c r="ZI34" s="0"/>
+      <c r="ZJ34" s="0"/>
+      <c r="ZK34" s="0"/>
+      <c r="ZL34" s="0"/>
+      <c r="ZM34" s="0"/>
+      <c r="ZN34" s="0"/>
+      <c r="ZO34" s="0"/>
+      <c r="ZP34" s="0"/>
+      <c r="ZQ34" s="0"/>
+      <c r="ZR34" s="0"/>
+      <c r="ZS34" s="0"/>
+      <c r="ZT34" s="0"/>
+      <c r="ZU34" s="0"/>
+      <c r="ZV34" s="0"/>
+      <c r="ZW34" s="0"/>
+      <c r="ZX34" s="0"/>
+      <c r="ZY34" s="0"/>
+      <c r="ZZ34" s="0"/>
+      <c r="AAA34" s="0"/>
+      <c r="AAB34" s="0"/>
+      <c r="AAC34" s="0"/>
+      <c r="AAD34" s="0"/>
+      <c r="AAE34" s="0"/>
+      <c r="AAF34" s="0"/>
+      <c r="AAG34" s="0"/>
+      <c r="AAH34" s="0"/>
+      <c r="AAI34" s="0"/>
+      <c r="AAJ34" s="0"/>
+      <c r="AAK34" s="0"/>
+      <c r="AAL34" s="0"/>
+      <c r="AAM34" s="0"/>
+      <c r="AAN34" s="0"/>
+      <c r="AAO34" s="0"/>
+      <c r="AAP34" s="0"/>
+      <c r="AAQ34" s="0"/>
+      <c r="AAR34" s="0"/>
+      <c r="AAS34" s="0"/>
+      <c r="AAT34" s="0"/>
+      <c r="AAU34" s="0"/>
+      <c r="AAV34" s="0"/>
+      <c r="AAW34" s="0"/>
+      <c r="AAX34" s="0"/>
+      <c r="AAY34" s="0"/>
+      <c r="AAZ34" s="0"/>
+      <c r="ABA34" s="0"/>
+      <c r="ABB34" s="0"/>
+      <c r="ABC34" s="0"/>
+      <c r="ABD34" s="0"/>
+      <c r="ABE34" s="0"/>
+      <c r="ABF34" s="0"/>
+      <c r="ABG34" s="0"/>
+      <c r="ABH34" s="0"/>
+      <c r="ABI34" s="0"/>
+      <c r="ABJ34" s="0"/>
+      <c r="ABK34" s="0"/>
+      <c r="ABL34" s="0"/>
+      <c r="ABM34" s="0"/>
+      <c r="ABN34" s="0"/>
+      <c r="ABO34" s="0"/>
+      <c r="ABP34" s="0"/>
+      <c r="ABQ34" s="0"/>
+      <c r="ABR34" s="0"/>
+      <c r="ABS34" s="0"/>
+      <c r="ABT34" s="0"/>
+      <c r="ABU34" s="0"/>
+      <c r="ABV34" s="0"/>
+      <c r="ABW34" s="0"/>
+      <c r="ABX34" s="0"/>
+      <c r="ABY34" s="0"/>
+      <c r="ABZ34" s="0"/>
+      <c r="ACA34" s="0"/>
+      <c r="ACB34" s="0"/>
+      <c r="ACC34" s="0"/>
+      <c r="ACD34" s="0"/>
+      <c r="ACE34" s="0"/>
+      <c r="ACF34" s="0"/>
+      <c r="ACG34" s="0"/>
+      <c r="ACH34" s="0"/>
+      <c r="ACI34" s="0"/>
+      <c r="ACJ34" s="0"/>
+      <c r="ACK34" s="0"/>
+      <c r="ACL34" s="0"/>
+      <c r="ACM34" s="0"/>
+      <c r="ACN34" s="0"/>
+      <c r="ACO34" s="0"/>
+      <c r="ACP34" s="0"/>
+      <c r="ACQ34" s="0"/>
+      <c r="ACR34" s="0"/>
+      <c r="ACS34" s="0"/>
+      <c r="ACT34" s="0"/>
+      <c r="ACU34" s="0"/>
+      <c r="ACV34" s="0"/>
+      <c r="ACW34" s="0"/>
+      <c r="ACX34" s="0"/>
+      <c r="ACY34" s="0"/>
+      <c r="ACZ34" s="0"/>
+      <c r="ADA34" s="0"/>
+      <c r="ADB34" s="0"/>
+      <c r="ADC34" s="0"/>
+      <c r="ADD34" s="0"/>
+      <c r="ADE34" s="0"/>
+      <c r="ADF34" s="0"/>
+      <c r="ADG34" s="0"/>
+      <c r="ADH34" s="0"/>
+      <c r="ADI34" s="0"/>
+      <c r="ADJ34" s="0"/>
+      <c r="ADK34" s="0"/>
+      <c r="ADL34" s="0"/>
+      <c r="ADM34" s="0"/>
+      <c r="ADN34" s="0"/>
+      <c r="ADO34" s="0"/>
+      <c r="ADP34" s="0"/>
+      <c r="ADQ34" s="0"/>
+      <c r="ADR34" s="0"/>
+      <c r="ADS34" s="0"/>
+      <c r="ADT34" s="0"/>
+      <c r="ADU34" s="0"/>
+      <c r="ADV34" s="0"/>
+      <c r="ADW34" s="0"/>
+      <c r="ADX34" s="0"/>
+      <c r="ADY34" s="0"/>
+      <c r="ADZ34" s="0"/>
+      <c r="AEA34" s="0"/>
+      <c r="AEB34" s="0"/>
+      <c r="AEC34" s="0"/>
+      <c r="AED34" s="0"/>
+      <c r="AEE34" s="0"/>
+      <c r="AEF34" s="0"/>
+      <c r="AEG34" s="0"/>
+      <c r="AEH34" s="0"/>
+      <c r="AEI34" s="0"/>
+      <c r="AEJ34" s="0"/>
+      <c r="AEK34" s="0"/>
+      <c r="AEL34" s="0"/>
+      <c r="AEM34" s="0"/>
+      <c r="AEN34" s="0"/>
+      <c r="AEO34" s="0"/>
+      <c r="AEP34" s="0"/>
+      <c r="AEQ34" s="0"/>
+      <c r="AER34" s="0"/>
+      <c r="AES34" s="0"/>
+      <c r="AET34" s="0"/>
+      <c r="AEU34" s="0"/>
+      <c r="AEV34" s="0"/>
+      <c r="AEW34" s="0"/>
+      <c r="AEX34" s="0"/>
+      <c r="AEY34" s="0"/>
+      <c r="AEZ34" s="0"/>
+      <c r="AFA34" s="0"/>
+      <c r="AFB34" s="0"/>
+      <c r="AFC34" s="0"/>
+      <c r="AFD34" s="0"/>
+      <c r="AFE34" s="0"/>
+      <c r="AFF34" s="0"/>
+      <c r="AFG34" s="0"/>
+      <c r="AFH34" s="0"/>
+      <c r="AFI34" s="0"/>
+      <c r="AFJ34" s="0"/>
+      <c r="AFK34" s="0"/>
+      <c r="AFL34" s="0"/>
+      <c r="AFM34" s="0"/>
+      <c r="AFN34" s="0"/>
+      <c r="AFO34" s="0"/>
+      <c r="AFP34" s="0"/>
+      <c r="AFQ34" s="0"/>
+      <c r="AFR34" s="0"/>
+      <c r="AFS34" s="0"/>
+      <c r="AFT34" s="0"/>
+      <c r="AFU34" s="0"/>
+      <c r="AFV34" s="0"/>
+      <c r="AFW34" s="0"/>
+      <c r="AFX34" s="0"/>
+      <c r="AFY34" s="0"/>
+      <c r="AFZ34" s="0"/>
+      <c r="AGA34" s="0"/>
+      <c r="AGB34" s="0"/>
+      <c r="AGC34" s="0"/>
+      <c r="AGD34" s="0"/>
+      <c r="AGE34" s="0"/>
+      <c r="AGF34" s="0"/>
+      <c r="AGG34" s="0"/>
+      <c r="AGH34" s="0"/>
+      <c r="AGI34" s="0"/>
+      <c r="AGJ34" s="0"/>
+      <c r="AGK34" s="0"/>
+      <c r="AGL34" s="0"/>
+      <c r="AGM34" s="0"/>
+      <c r="AGN34" s="0"/>
+      <c r="AGO34" s="0"/>
+      <c r="AGP34" s="0"/>
+      <c r="AGQ34" s="0"/>
+      <c r="AGR34" s="0"/>
+      <c r="AGS34" s="0"/>
+      <c r="AGT34" s="0"/>
+      <c r="AGU34" s="0"/>
+      <c r="AGV34" s="0"/>
+      <c r="AGW34" s="0"/>
+      <c r="AGX34" s="0"/>
+      <c r="AGY34" s="0"/>
+      <c r="AGZ34" s="0"/>
+      <c r="AHA34" s="0"/>
+      <c r="AHB34" s="0"/>
+      <c r="AHC34" s="0"/>
+      <c r="AHD34" s="0"/>
+      <c r="AHE34" s="0"/>
+      <c r="AHF34" s="0"/>
+      <c r="AHG34" s="0"/>
+      <c r="AHH34" s="0"/>
+      <c r="AHI34" s="0"/>
+      <c r="AHJ34" s="0"/>
+      <c r="AHK34" s="0"/>
+      <c r="AHL34" s="0"/>
+      <c r="AHM34" s="0"/>
+      <c r="AHN34" s="0"/>
+      <c r="AHO34" s="0"/>
+      <c r="AHP34" s="0"/>
+      <c r="AHQ34" s="0"/>
+      <c r="AHR34" s="0"/>
+      <c r="AHS34" s="0"/>
+      <c r="AHT34" s="0"/>
+      <c r="AHU34" s="0"/>
+      <c r="AHV34" s="0"/>
+      <c r="AHW34" s="0"/>
+      <c r="AHX34" s="0"/>
+      <c r="AHY34" s="0"/>
+      <c r="AHZ34" s="0"/>
+      <c r="AIA34" s="0"/>
+      <c r="AIB34" s="0"/>
+      <c r="AIC34" s="0"/>
+      <c r="AID34" s="0"/>
+      <c r="AIE34" s="0"/>
+      <c r="AIF34" s="0"/>
+      <c r="AIG34" s="0"/>
+      <c r="AIH34" s="0"/>
+      <c r="AII34" s="0"/>
+      <c r="AIJ34" s="0"/>
+      <c r="AIK34" s="0"/>
+      <c r="AIL34" s="0"/>
+      <c r="AIM34" s="0"/>
+      <c r="AIN34" s="0"/>
+      <c r="AIO34" s="0"/>
+      <c r="AIP34" s="0"/>
+      <c r="AIQ34" s="0"/>
+      <c r="AIR34" s="0"/>
+      <c r="AIS34" s="0"/>
+      <c r="AIT34" s="0"/>
+      <c r="AIU34" s="0"/>
+      <c r="AIV34" s="0"/>
+      <c r="AIW34" s="0"/>
+      <c r="AIX34" s="0"/>
+      <c r="AIY34" s="0"/>
+      <c r="AIZ34" s="0"/>
+      <c r="AJA34" s="0"/>
+      <c r="AJB34" s="0"/>
+      <c r="AJC34" s="0"/>
+      <c r="AJD34" s="0"/>
+      <c r="AJE34" s="0"/>
+      <c r="AJF34" s="0"/>
+      <c r="AJG34" s="0"/>
+      <c r="AJH34" s="0"/>
+      <c r="AJI34" s="0"/>
+      <c r="AJJ34" s="0"/>
+      <c r="AJK34" s="0"/>
+      <c r="AJL34" s="0"/>
+      <c r="AJM34" s="0"/>
+      <c r="AJN34" s="0"/>
+      <c r="AJO34" s="0"/>
+      <c r="AJP34" s="0"/>
+      <c r="AJQ34" s="0"/>
+      <c r="AJR34" s="0"/>
+      <c r="AJS34" s="0"/>
+      <c r="AJT34" s="0"/>
+      <c r="AJU34" s="0"/>
+      <c r="AJV34" s="0"/>
+      <c r="AJW34" s="0"/>
+      <c r="AJX34" s="0"/>
+      <c r="AJY34" s="0"/>
+      <c r="AJZ34" s="0"/>
+      <c r="AKA34" s="0"/>
+      <c r="AKB34" s="0"/>
+      <c r="AKC34" s="0"/>
+      <c r="AKD34" s="0"/>
+      <c r="AKE34" s="0"/>
+      <c r="AKF34" s="0"/>
+      <c r="AKG34" s="0"/>
+      <c r="AKH34" s="0"/>
+      <c r="AKI34" s="0"/>
+      <c r="AKJ34" s="0"/>
+      <c r="AKK34" s="0"/>
+      <c r="AKL34" s="0"/>
+      <c r="AKM34" s="0"/>
+      <c r="AKN34" s="0"/>
+      <c r="AKO34" s="0"/>
+      <c r="AKP34" s="0"/>
+      <c r="AKQ34" s="0"/>
+      <c r="AKR34" s="0"/>
+      <c r="AKS34" s="0"/>
+      <c r="AKT34" s="0"/>
+      <c r="AKU34" s="0"/>
+      <c r="AKV34" s="0"/>
+      <c r="AKW34" s="0"/>
+      <c r="AKX34" s="0"/>
+      <c r="AKY34" s="0"/>
+      <c r="AKZ34" s="0"/>
+      <c r="ALA34" s="0"/>
+      <c r="ALB34" s="0"/>
+      <c r="ALC34" s="0"/>
+      <c r="ALD34" s="0"/>
+      <c r="ALE34" s="0"/>
+      <c r="ALF34" s="0"/>
+      <c r="ALG34" s="0"/>
+      <c r="ALH34" s="0"/>
+      <c r="ALI34" s="0"/>
+      <c r="ALJ34" s="0"/>
+      <c r="ALK34" s="0"/>
+      <c r="ALL34" s="0"/>
+      <c r="ALM34" s="0"/>
+      <c r="ALN34" s="0"/>
+      <c r="ALO34" s="0"/>
+      <c r="ALP34" s="0"/>
+      <c r="ALQ34" s="0"/>
+      <c r="ALR34" s="0"/>
+      <c r="ALS34" s="0"/>
+      <c r="ALT34" s="0"/>
+      <c r="ALU34" s="0"/>
+      <c r="ALV34" s="0"/>
+      <c r="ALW34" s="0"/>
+      <c r="ALX34" s="0"/>
+      <c r="ALY34" s="0"/>
+      <c r="ALZ34" s="0"/>
+      <c r="AMA34" s="0"/>
+      <c r="AMB34" s="0"/>
+      <c r="AMC34" s="0"/>
+      <c r="AMD34" s="0"/>
+      <c r="AME34" s="0"/>
+      <c r="AMF34" s="0"/>
+      <c r="AMG34" s="0"/>
+      <c r="AMH34" s="0"/>
+      <c r="AMI34" s="0"/>
+      <c r="AMJ34" s="0"/>
+    </row>
+    <row r="38" s="136" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="137"/>
+      <c r="D38" s="137"/>
       <c r="G38" s="56"/>
       <c r="H38" s="56"/>
       <c r="I38" s="56"/>
@@ -52401,9 +55596,9 @@
       <c r="AE38" s="56"/>
       <c r="AF38" s="56"/>
     </row>
-    <row r="39" s="129" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="130"/>
-      <c r="D39" s="130"/>
+    <row r="39" s="136" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="137"/>
+      <c r="D39" s="137"/>
       <c r="G39" s="56"/>
       <c r="H39" s="56"/>
       <c r="I39" s="56"/>
@@ -52431,9 +55626,9 @@
       <c r="AE39" s="56"/>
       <c r="AF39" s="56"/>
     </row>
-    <row r="40" s="129" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="130"/>
-      <c r="D40" s="130"/>
+    <row r="40" s="136" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="137"/>
+      <c r="D40" s="137"/>
       <c r="G40" s="56"/>
       <c r="H40" s="56"/>
       <c r="I40" s="56"/>
@@ -52462,10 +55657,10 @@
       <c r="AF40" s="56"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="129"/>
-      <c r="B41" s="129"/>
-      <c r="C41" s="131"/>
-      <c r="D41" s="131"/>
+      <c r="A41" s="136"/>
+      <c r="B41" s="136"/>
+      <c r="C41" s="138"/>
+      <c r="D41" s="138"/>
       <c r="G41" s="56"/>
       <c r="H41" s="56"/>
       <c r="I41" s="56"/>
@@ -52494,10 +55689,10 @@
       <c r="AF41" s="56"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="129"/>
-      <c r="B42" s="129"/>
-      <c r="C42" s="131"/>
-      <c r="D42" s="131"/>
+      <c r="A42" s="136"/>
+      <c r="B42" s="136"/>
+      <c r="C42" s="138"/>
+      <c r="D42" s="138"/>
       <c r="G42" s="56"/>
       <c r="H42" s="56"/>
       <c r="I42" s="56"/>
@@ -52526,10 +55721,10 @@
       <c r="AF42" s="56"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="129"/>
-      <c r="B43" s="129"/>
-      <c r="C43" s="131"/>
-      <c r="D43" s="131"/>
+      <c r="A43" s="136"/>
+      <c r="B43" s="136"/>
+      <c r="C43" s="138"/>
+      <c r="D43" s="138"/>
       <c r="G43" s="56"/>
       <c r="H43" s="56"/>
       <c r="I43" s="56"/>

</xml_diff>